<commit_message>
testing automatic change log changes
</commit_message>
<xml_diff>
--- a/src/assets/database.xlsx
+++ b/src/assets/database.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{5955EB84-E635-41A3-9C81-2C8297675F9E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED24BCA-EA35-42EE-8CCF-85AD247DC49E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25840" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5200" yWindow="2290" windowWidth="19200" windowHeight="9980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ChangeLog" sheetId="11" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3494" uniqueCount="2097">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3496" uniqueCount="2099">
   <si>
     <t>id</t>
   </si>
@@ -7152,6 +7152,12 @@
   </si>
   <si>
     <t>Launch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pre Launch </t>
+  </si>
+  <si>
+    <t>Alex Li And Matt</t>
   </si>
 </sst>
 </file>
@@ -7565,7 +7571,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7600,14 +7606,22 @@
         <v>43874</v>
       </c>
       <c r="B3" t="s">
+        <v>2098</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2097</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="5">
+        <v>43874</v>
+      </c>
+      <c r="B4" t="s">
         <v>2095</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>2096</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20087,6 +20101,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_STS_x0020_Hashtags xmlns="b38e6452-0983-483a-b0d4-324af6d44e4d"/>
+    <MediaServiceKeyPoints xmlns="b38e6452-0983-483a-b0d4-324af6d44e4d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010072B72D3E1CFCDD40BC0C6D9CCD45E0BB" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1091b63e79dc81a90741573e3164413c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="759c4387-f01d-437d-8a5d-56d9b05a6914" xmlns:ns4="b38e6452-0983-483a-b0d4-324af6d44e4d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7010e408eae2039b0bc4bac303a742c1" ns3:_="" ns4:_="">
     <xsd:import namespace="759c4387-f01d-437d-8a5d-56d9b05a6914"/>
@@ -20337,15 +20360,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_STS_x0020_Hashtags xmlns="b38e6452-0983-483a-b0d4-324af6d44e4d"/>
-    <MediaServiceKeyPoints xmlns="b38e6452-0983-483a-b0d4-324af6d44e4d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A59176D2-D324-41A5-A125-AC358C249804}">
   <ds:schemaRefs>
@@ -20355,6 +20369,16 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71725466-609F-438E-9D55-68B1CE9C392F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b38e6452-0983-483a-b0d4-324af6d44e4d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC11F96C-E600-42F3-BB18-A579B8C44705}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20371,14 +20395,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71725466-609F-438E-9D55-68B1CE9C392F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b38e6452-0983-483a-b0d4-324af6d44e4d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
further data clean up
</commit_message>
<xml_diff>
--- a/src/assets/database.xlsx
+++ b/src/assets/database.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{719F5EC7-5D72-4677-9E50-863125BD9E64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B870772E-9DFB-4C9C-82DC-65823EEFD081}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5130" uniqueCount="2808">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5130" uniqueCount="2807">
   <si>
     <t>id</t>
   </si>
@@ -7614,9 +7614,6 @@
     <t>63 Procedure for adjudication by Adjudicating Officer</t>
   </si>
   <si>
-    <t>5.2.2.</t>
-  </si>
-  <si>
     <t>(1) For the purpose of adjudging the penalties under sections 57 to 61or awarding compensation under section 64, the Authority shall appoint such Adjudicating Officer as may be prescribed.
 (2)  The Central Government shall, having regard to the need to ensure the operational segregation, independence, and neutrality of the adjudication under this Act, prescribe—
 (a) number of Adjudicating Officers to be appointed under sub-section (1); 
@@ -9608,9 +9605,6 @@
     <t>7.3.2;7.3.3.;7.2.8;8.3.1;6.15.2</t>
   </si>
   <si>
-    <t>5.2.1;5.2.2.</t>
-  </si>
-  <si>
     <t>6.15.2.3;6.13.1;6.13.1.5</t>
   </si>
   <si>
@@ -9623,9 +9617,6 @@
     <t>7.2.4;7.2.2;8.2.1</t>
   </si>
   <si>
-    <t>6.4.1.2;7.2.2.</t>
-  </si>
-  <si>
     <t>7.3.8;7.3.9</t>
   </si>
   <si>
@@ -9665,9 +9656,6 @@
     <t>7.4.4;6.15.1.3;6.2.1.1;7.2.8</t>
   </si>
   <si>
-    <t>7.3.1;;7.3.2;7.3.3;</t>
-  </si>
-  <si>
     <t>7.2.2;5.3.2;5.2.1</t>
   </si>
   <si>
@@ -9699,6 +9687,15 @@
   </si>
   <si>
     <t>5.2.1;5.2.2;5.3.3;5.3.1</t>
+  </si>
+  <si>
+    <t>6.4.1.2;7.2.2</t>
+  </si>
+  <si>
+    <t>7.3.1;7.3.2;7.3.3;</t>
+  </si>
+  <si>
+    <t>5.2.1;5.2.2</t>
   </si>
 </sst>
 </file>
@@ -10230,7 +10227,7 @@
         <v>2090</v>
       </c>
       <c r="C4" t="s">
-        <v>2742</v>
+        <v>2741</v>
       </c>
     </row>
   </sheetData>
@@ -21724,8 +21721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24BA70E6-9548-4D87-8A65-060EC90D2814}">
   <dimension ref="A1:F664"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A189" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E355" sqref="E355"/>
+    <sheetView tabSelected="1" topLeftCell="A347" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E335" sqref="E335"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -21742,10 +21739,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2741</v>
+        <v>2740</v>
       </c>
       <c r="C1" t="s">
-        <v>2740</v>
+        <v>2739</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>3</v>
@@ -21754,7 +21751,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>2739</v>
+        <v>2738</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="153">
@@ -21762,13 +21759,13 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>2738</v>
+        <v>2737</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>2737</v>
+        <v>2736</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>2736</v>
+        <v>2735</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="105">
@@ -21776,17 +21773,17 @@
         <v>4</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>2735</v>
+        <v>2734</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>2734</v>
+        <v>2733</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="8" t="s">
-        <v>2743</v>
+        <v>2742</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>2733</v>
+        <v>2732</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="135">
@@ -21794,39 +21791,39 @@
         <v>5</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>2732</v>
+        <v>2731</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
     </row>
     <row r="5" spans="1:6" ht="30">
       <c r="A5" t="s">
-        <v>2731</v>
+        <v>2730</v>
       </c>
       <c r="B5" t="s">
-        <v>2731</v>
+        <v>2730</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>2730</v>
+        <v>2729</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="8" t="s">
-        <v>2789</v>
+        <v>2786</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="51">
       <c r="A6" t="s">
-        <v>2729</v>
+        <v>2728</v>
       </c>
       <c r="B6" t="s">
-        <v>2729</v>
+        <v>2728</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>2728</v>
+        <v>2727</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="8" t="s">
-        <v>2790</v>
+        <v>2787</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="105">
@@ -21834,10 +21831,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>2727</v>
+        <v>2726</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>2726</v>
+        <v>2725</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="8" t="s">
@@ -21849,7 +21846,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>2725</v>
+        <v>2724</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -21862,22 +21859,22 @@
         <v>7.1</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>2724</v>
+        <v>2723</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="8" t="s">
-        <v>2744</v>
+        <v>2743</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>2723</v>
+        <v>2722</v>
       </c>
       <c r="B10" t="s">
-        <v>2723</v>
+        <v>2722</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>2722</v>
+        <v>2721</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="8" t="s">
@@ -21886,13 +21883,13 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>2721</v>
+        <v>2720</v>
       </c>
       <c r="B11" t="s">
-        <v>2721</v>
+        <v>2720</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>2720</v>
+        <v>2719</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="8" t="s">
@@ -21901,13 +21898,13 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>2719</v>
+        <v>2718</v>
       </c>
       <c r="B12" t="s">
-        <v>2719</v>
+        <v>2718</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>2718</v>
+        <v>2717</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="8" t="s">
@@ -21916,13 +21913,13 @@
     </row>
     <row r="13" spans="1:6" ht="25.5">
       <c r="A13" t="s">
-        <v>2717</v>
+        <v>2716</v>
       </c>
       <c r="B13" t="s">
-        <v>2717</v>
+        <v>2716</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>2716</v>
+        <v>2715</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="8" t="s">
@@ -21931,13 +21928,13 @@
     </row>
     <row r="14" spans="1:6" ht="29.1" customHeight="1">
       <c r="A14" t="s">
-        <v>2715</v>
+        <v>2714</v>
       </c>
       <c r="B14" t="s">
-        <v>2715</v>
+        <v>2714</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>2714</v>
+        <v>2713</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="8" t="s">
@@ -21946,13 +21943,13 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>2713</v>
+        <v>2712</v>
       </c>
       <c r="B15" t="s">
-        <v>2713</v>
+        <v>2712</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>2712</v>
+        <v>2711</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="8" t="s">
@@ -21961,31 +21958,31 @@
     </row>
     <row r="16" spans="1:6" ht="30">
       <c r="A16" t="s">
-        <v>2711</v>
+        <v>2710</v>
       </c>
       <c r="B16" t="s">
-        <v>2711</v>
+        <v>2710</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>2710</v>
+        <v>2709</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="8" t="s">
         <v>673</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>2709</v>
+        <v>2708</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="25.5">
       <c r="A17" t="s">
-        <v>2708</v>
+        <v>2707</v>
       </c>
       <c r="B17" t="s">
-        <v>2708</v>
+        <v>2707</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>2707</v>
+        <v>2706</v>
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="8" t="s">
@@ -21994,13 +21991,13 @@
     </row>
     <row r="18" spans="1:6" ht="25.5">
       <c r="A18" t="s">
-        <v>2706</v>
+        <v>2705</v>
       </c>
       <c r="B18" t="s">
-        <v>2706</v>
+        <v>2705</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>2705</v>
+        <v>2704</v>
       </c>
       <c r="D18" s="10"/>
       <c r="E18" s="8" t="s">
@@ -22009,13 +22006,13 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>2704</v>
+        <v>2703</v>
       </c>
       <c r="B19" t="s">
-        <v>2704</v>
+        <v>2703</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>2703</v>
+        <v>2702</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="8" t="s">
@@ -22024,58 +22021,58 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>2702</v>
+        <v>2701</v>
       </c>
       <c r="B20" t="s">
-        <v>2702</v>
+        <v>2701</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>2701</v>
+        <v>2700</v>
       </c>
       <c r="D20" s="10"/>
       <c r="F20" s="8" t="s">
-        <v>2696</v>
+        <v>2695</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>2700</v>
+        <v>2699</v>
       </c>
       <c r="B21" t="s">
-        <v>2700</v>
+        <v>2699</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>2699</v>
+        <v>2698</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="8" t="s">
-        <v>2745</v>
+        <v>2744</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="25.5">
       <c r="A22" t="s">
-        <v>2698</v>
+        <v>2697</v>
       </c>
       <c r="B22" t="s">
-        <v>2698</v>
+        <v>2697</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>2697</v>
+        <v>2696</v>
       </c>
       <c r="D22" s="10"/>
       <c r="F22" s="8" t="s">
-        <v>2696</v>
+        <v>2695</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1">
       <c r="A23" t="s">
-        <v>2695</v>
+        <v>2694</v>
       </c>
       <c r="B23" t="s">
-        <v>2695</v>
+        <v>2694</v>
       </c>
       <c r="C23" t="s">
-        <v>2694</v>
+        <v>2693</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="30">
@@ -22086,14 +22083,14 @@
         <v>7.2</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>2693</v>
+        <v>2692</v>
       </c>
       <c r="D24" s="10"/>
       <c r="E24" s="8" t="s">
         <v>187</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>2692</v>
+        <v>2691</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="25.5">
@@ -22104,11 +22101,11 @@
         <v>7.3</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>2691</v>
+        <v>2690</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="8" t="s">
-        <v>2746</v>
+        <v>2745</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="90">
@@ -22116,7 +22113,7 @@
         <v>8</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>2690</v>
+        <v>2689</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
@@ -22129,55 +22126,55 @@
         <v>8.1</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>2689</v>
+        <v>2688</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="8" t="s">
         <v>221</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>2688</v>
+        <v>2687</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="25.5">
       <c r="A28" t="s">
-        <v>2687</v>
+        <v>2686</v>
       </c>
       <c r="B28" t="s">
-        <v>2687</v>
+        <v>2686</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>2686</v>
+        <v>2685</v>
       </c>
       <c r="D28" s="10"/>
       <c r="E28" s="8" t="s">
-        <v>2747</v>
+        <v>2746</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>2685</v>
+        <v>2684</v>
       </c>
       <c r="B29" t="s">
-        <v>2685</v>
+        <v>2684</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>2684</v>
+        <v>2683</v>
       </c>
       <c r="D29" s="10"/>
       <c r="E29" s="8" t="s">
-        <v>2748</v>
+        <v>2747</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="25.5">
       <c r="A30" t="s">
-        <v>2683</v>
+        <v>2682</v>
       </c>
       <c r="B30" t="s">
-        <v>2683</v>
+        <v>2682</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>2682</v>
+        <v>2681</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30" s="8" t="s">
@@ -22192,11 +22189,11 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>2681</v>
+        <v>2680</v>
       </c>
       <c r="D31" s="10"/>
       <c r="E31" s="8" t="s">
-        <v>2749</v>
+        <v>2748</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="42.95" customHeight="1">
@@ -22204,7 +22201,7 @@
         <v>9</v>
       </c>
       <c r="B32" t="s">
-        <v>2680</v>
+        <v>2679</v>
       </c>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
@@ -22217,14 +22214,14 @@
         <v>9.1</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>2679</v>
+        <v>2678</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="8" t="s">
-        <v>2791</v>
+        <v>2788</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>2678</v>
+        <v>2677</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="28.5" customHeight="1">
@@ -22235,7 +22232,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>2677</v>
+        <v>2676</v>
       </c>
       <c r="D34" s="10"/>
       <c r="E34" s="8" t="s">
@@ -22250,11 +22247,11 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>2676</v>
+        <v>2675</v>
       </c>
       <c r="D35" s="10"/>
       <c r="E35" s="8" t="s">
-        <v>2750</v>
+        <v>2749</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="31.5" customHeight="1">
@@ -22265,11 +22262,11 @@
         <v>9.4</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>2675</v>
+        <v>2674</v>
       </c>
       <c r="D36" s="10"/>
       <c r="E36" s="8" t="s">
-        <v>2780</v>
+        <v>2778</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="75">
@@ -22277,10 +22274,10 @@
         <v>10</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>2674</v>
+        <v>2673</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>2673</v>
+        <v>2672</v>
       </c>
       <c r="D37" s="10"/>
       <c r="E37" s="8" t="s">
@@ -22292,7 +22289,7 @@
         <v>11</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>2672</v>
+        <v>2671</v>
       </c>
       <c r="C38" s="10"/>
       <c r="D38" s="10"/>
@@ -22305,7 +22302,7 @@
         <v>11.1</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>2671</v>
+        <v>2670</v>
       </c>
       <c r="D39" s="10"/>
       <c r="E39" s="8" t="s">
@@ -22314,115 +22311,115 @@
     </row>
     <row r="40" spans="1:6" ht="60">
       <c r="A40" t="s">
-        <v>2670</v>
+        <v>2669</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>2670</v>
+        <v>2669</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>2669</v>
+        <v>2668</v>
       </c>
       <c r="D40" s="10"/>
       <c r="E40" s="8" t="s">
-        <v>2781</v>
+        <v>2779</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>2668</v>
+        <v>2667</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="45">
       <c r="A41" t="s">
-        <v>2667</v>
+        <v>2666</v>
       </c>
       <c r="B41" t="s">
-        <v>2667</v>
+        <v>2666</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>2666</v>
+        <v>2665</v>
       </c>
       <c r="D41" s="10"/>
       <c r="E41" s="8" t="s">
         <v>165</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>2665</v>
+        <v>2664</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="25.5">
       <c r="A42" t="s">
-        <v>2664</v>
+        <v>2663</v>
       </c>
       <c r="B42" t="s">
-        <v>2664</v>
+        <v>2663</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>2663</v>
+        <v>2662</v>
       </c>
       <c r="D42" s="10"/>
       <c r="E42" s="8" t="s">
         <v>165</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>2662</v>
+        <v>2661</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>2661</v>
+        <v>2660</v>
       </c>
       <c r="B43" t="s">
-        <v>2661</v>
+        <v>2660</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>2660</v>
+        <v>2659</v>
       </c>
       <c r="D43" s="10"/>
       <c r="E43" s="8" t="s">
         <v>165</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>2659</v>
+        <v>2658</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="28.5" customHeight="1">
       <c r="A44" t="s">
-        <v>2658</v>
+        <v>2657</v>
       </c>
       <c r="B44" t="s">
-        <v>2658</v>
+        <v>2657</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>2657</v>
+        <v>2656</v>
       </c>
       <c r="D44" s="10"/>
       <c r="E44" s="8" t="s">
-        <v>2751</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="39.6" customHeight="1">
       <c r="A45" t="s">
-        <v>2656</v>
+        <v>2655</v>
       </c>
       <c r="B45" t="s">
-        <v>2656</v>
+        <v>2655</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>2655</v>
+        <v>2654</v>
       </c>
       <c r="D45" s="10"/>
       <c r="E45" s="8" t="s">
-        <v>2752</v>
+        <v>2751</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>2654</v>
+        <v>2653</v>
       </c>
       <c r="B46" t="s">
-        <v>2654</v>
+        <v>2653</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>2653</v>
+        <v>2652</v>
       </c>
       <c r="D46" s="10"/>
       <c r="E46" s="8" t="s">
@@ -22431,13 +22428,13 @@
     </row>
     <row r="47" spans="1:6" ht="30" customHeight="1">
       <c r="A47" t="s">
-        <v>2652</v>
+        <v>2651</v>
       </c>
       <c r="B47" t="s">
-        <v>2652</v>
+        <v>2651</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>2651</v>
+        <v>2650</v>
       </c>
       <c r="D47" s="10"/>
       <c r="E47" s="8" t="s">
@@ -22452,14 +22449,14 @@
         <v>11.4</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>2650</v>
+        <v>2649</v>
       </c>
       <c r="D48" s="10"/>
       <c r="E48" s="8" t="s">
         <v>159</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>2649</v>
+        <v>2648</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="30" customHeight="1">
@@ -22470,7 +22467,7 @@
         <v>11.5</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>2648</v>
+        <v>2647</v>
       </c>
       <c r="D49" s="10"/>
       <c r="E49" s="8" t="s">
@@ -22485,11 +22482,11 @@
         <v>11.6</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>2647</v>
+        <v>2646</v>
       </c>
       <c r="D50" s="10"/>
       <c r="F50" s="8" t="s">
-        <v>2646</v>
+        <v>2645</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="33.6" customHeight="1">
@@ -22497,38 +22494,38 @@
         <v>12</v>
       </c>
       <c r="B51" t="s">
-        <v>2645</v>
+        <v>2644</v>
       </c>
       <c r="C51" s="10"/>
       <c r="D51" s="10"/>
     </row>
     <row r="52" spans="1:6" ht="42.95" customHeight="1">
       <c r="A52" t="s">
-        <v>2644</v>
+        <v>2643</v>
       </c>
       <c r="B52" t="s">
-        <v>2644</v>
+        <v>2643</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>2643</v>
+        <v>2642</v>
       </c>
       <c r="D52" s="10"/>
       <c r="E52" s="8" t="s">
         <v>159</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>2642</v>
+        <v>2641</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>2641</v>
+        <v>2640</v>
       </c>
       <c r="B53" t="s">
-        <v>2641</v>
+        <v>2640</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>2640</v>
+        <v>2639</v>
       </c>
       <c r="D53" s="10"/>
       <c r="E53" s="8" t="s">
@@ -22537,13 +22534,13 @@
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>2639</v>
+        <v>2638</v>
       </c>
       <c r="B54" t="s">
-        <v>2639</v>
+        <v>2638</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>2638</v>
+        <v>2637</v>
       </c>
       <c r="D54" s="10"/>
       <c r="E54" s="8" t="s">
@@ -22552,25 +22549,25 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>2637</v>
+        <v>2636</v>
       </c>
       <c r="B55" t="s">
-        <v>2637</v>
+        <v>2636</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>2636</v>
+        <v>2635</v>
       </c>
       <c r="D55" s="10"/>
     </row>
     <row r="56" spans="1:6" ht="25.5">
       <c r="A56" t="s">
-        <v>2635</v>
+        <v>2634</v>
       </c>
       <c r="B56" t="s">
-        <v>2635</v>
+        <v>2634</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>2634</v>
+        <v>2633</v>
       </c>
       <c r="D56" s="10"/>
       <c r="E56" s="8" t="s">
@@ -22579,13 +22576,13 @@
     </row>
     <row r="57" spans="1:6" ht="25.5">
       <c r="A57" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="B57" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
       <c r="D57" s="10"/>
       <c r="E57" s="8" t="s">
@@ -22594,13 +22591,13 @@
     </row>
     <row r="58" spans="1:6" ht="24.95" customHeight="1">
       <c r="A58" t="s">
-        <v>2631</v>
+        <v>2630</v>
       </c>
       <c r="B58" t="s">
-        <v>2631</v>
+        <v>2630</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>2630</v>
+        <v>2629</v>
       </c>
       <c r="D58" s="10"/>
       <c r="E58" s="8" t="s">
@@ -22612,7 +22609,7 @@
         <v>13</v>
       </c>
       <c r="B59" t="s">
-        <v>2629</v>
+        <v>2628</v>
       </c>
       <c r="C59" s="10"/>
       <c r="D59" s="10"/>
@@ -22625,14 +22622,14 @@
         <v>684</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>2628</v>
+        <v>2627</v>
       </c>
       <c r="D60" s="10"/>
       <c r="E60" s="8" t="s">
-        <v>2782</v>
+        <v>2804</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>2627</v>
+        <v>2626</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -22643,11 +22640,11 @@
         <v>685</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>2626</v>
+        <v>2625</v>
       </c>
       <c r="D61" s="10"/>
       <c r="E61" s="8" t="s">
-        <v>2580</v>
+        <v>159</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -22658,11 +22655,11 @@
         <v>686</v>
       </c>
       <c r="C62" s="10" t="s">
-        <v>2625</v>
+        <v>2624</v>
       </c>
       <c r="D62" s="10"/>
       <c r="E62" s="8" t="s">
-        <v>2580</v>
+        <v>159</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="25.5">
@@ -22673,11 +22670,11 @@
         <v>687</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>2624</v>
+        <v>2623</v>
       </c>
       <c r="D63" s="10"/>
       <c r="E63" s="8" t="s">
-        <v>2580</v>
+        <v>159</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="51">
@@ -22688,11 +22685,11 @@
         <v>13.2</v>
       </c>
       <c r="C64" s="10" t="s">
-        <v>2623</v>
+        <v>2622</v>
       </c>
       <c r="D64" s="10"/>
       <c r="E64" s="8" t="s">
-        <v>2580</v>
+        <v>159</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -22700,7 +22697,7 @@
         <v>14</v>
       </c>
       <c r="B65" t="s">
-        <v>2622</v>
+        <v>2621</v>
       </c>
       <c r="C65" s="10"/>
       <c r="D65" s="10"/>
@@ -22713,14 +22710,14 @@
         <v>704</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>2621</v>
+        <v>2620</v>
       </c>
       <c r="D66" s="10"/>
       <c r="E66" s="8" t="s">
-        <v>2580</v>
+        <v>159</v>
       </c>
       <c r="F66" s="8" t="s">
-        <v>2620</v>
+        <v>2619</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="45">
@@ -22731,11 +22728,11 @@
         <v>705</v>
       </c>
       <c r="C67" s="10" t="s">
-        <v>2619</v>
+        <v>2618</v>
       </c>
       <c r="D67" s="10"/>
       <c r="F67" s="8" t="s">
-        <v>2618</v>
+        <v>2617</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -22746,7 +22743,7 @@
         <v>706</v>
       </c>
       <c r="C68" s="10" t="s">
-        <v>2617</v>
+        <v>2616</v>
       </c>
       <c r="D68" s="10"/>
       <c r="E68" s="8" t="s">
@@ -22761,7 +22758,7 @@
         <v>707</v>
       </c>
       <c r="C69" s="10" t="s">
-        <v>2616</v>
+        <v>2615</v>
       </c>
       <c r="D69" s="10"/>
       <c r="E69" s="8" t="s">
@@ -22776,7 +22773,7 @@
         <v>708</v>
       </c>
       <c r="C70" s="10" t="s">
-        <v>2615</v>
+        <v>2614</v>
       </c>
       <c r="D70" s="10"/>
     </row>
@@ -22788,11 +22785,11 @@
         <v>14.2</v>
       </c>
       <c r="C71" s="10" t="s">
-        <v>2614</v>
+        <v>2613</v>
       </c>
       <c r="D71" s="10"/>
       <c r="F71" s="8" t="s">
-        <v>2613</v>
+        <v>2612</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -22803,7 +22800,7 @@
         <v>711</v>
       </c>
       <c r="C72" s="10" t="s">
-        <v>2612</v>
+        <v>2611</v>
       </c>
       <c r="D72" s="10"/>
     </row>
@@ -22815,7 +22812,7 @@
         <v>712</v>
       </c>
       <c r="C73" s="10" t="s">
-        <v>2611</v>
+        <v>2610</v>
       </c>
       <c r="D73" s="10"/>
     </row>
@@ -22827,7 +22824,7 @@
         <v>713</v>
       </c>
       <c r="C74" s="10" t="s">
-        <v>2610</v>
+        <v>2609</v>
       </c>
       <c r="D74" s="10"/>
     </row>
@@ -22839,7 +22836,7 @@
         <v>714</v>
       </c>
       <c r="C75" s="10" t="s">
-        <v>2609</v>
+        <v>2608</v>
       </c>
       <c r="D75" s="10"/>
     </row>
@@ -22851,7 +22848,7 @@
         <v>715</v>
       </c>
       <c r="C76" s="10" t="s">
-        <v>2608</v>
+        <v>2607</v>
       </c>
       <c r="D76" s="10"/>
     </row>
@@ -22863,7 +22860,7 @@
         <v>716</v>
       </c>
       <c r="C77" s="10" t="s">
-        <v>2607</v>
+        <v>2606</v>
       </c>
       <c r="D77" s="10"/>
     </row>
@@ -22875,19 +22872,19 @@
         <v>717</v>
       </c>
       <c r="C78" s="10" t="s">
-        <v>2606</v>
+        <v>2605</v>
       </c>
       <c r="D78" s="10"/>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" t="s">
-        <v>2605</v>
+        <v>2604</v>
       </c>
       <c r="B79" t="s">
-        <v>2605</v>
+        <v>2604</v>
       </c>
       <c r="C79" s="10" t="s">
-        <v>2604</v>
+        <v>2603</v>
       </c>
       <c r="D79" s="10"/>
     </row>
@@ -22899,7 +22896,7 @@
         <v>14.3</v>
       </c>
       <c r="C80" s="10" t="s">
-        <v>2603</v>
+        <v>2602</v>
       </c>
       <c r="D80" s="10"/>
       <c r="E80" s="8" t="s">
@@ -22914,7 +22911,7 @@
         <v>705</v>
       </c>
       <c r="C81" s="10" t="s">
-        <v>2602</v>
+        <v>2601</v>
       </c>
       <c r="D81" s="10"/>
     </row>
@@ -22923,7 +22920,7 @@
         <v>15</v>
       </c>
       <c r="B82" t="s">
-        <v>2601</v>
+        <v>2600</v>
       </c>
       <c r="C82" s="10"/>
       <c r="D82" s="10"/>
@@ -22936,7 +22933,7 @@
         <v>731</v>
       </c>
       <c r="C83" s="10" t="s">
-        <v>2600</v>
+        <v>2599</v>
       </c>
       <c r="D83" s="10"/>
       <c r="E83" s="8" t="s">
@@ -22951,7 +22948,7 @@
         <v>733</v>
       </c>
       <c r="C84" s="10" t="s">
-        <v>2599</v>
+        <v>2598</v>
       </c>
       <c r="D84" s="10"/>
       <c r="E84" s="8" t="s">
@@ -22966,7 +22963,7 @@
         <v>734</v>
       </c>
       <c r="C85" s="10" t="s">
-        <v>2598</v>
+        <v>2597</v>
       </c>
       <c r="D85" s="10"/>
       <c r="E85" s="8" t="s">
@@ -22981,7 +22978,7 @@
         <v>735</v>
       </c>
       <c r="C86" s="10" t="s">
-        <v>2597</v>
+        <v>2596</v>
       </c>
       <c r="D86" s="10"/>
       <c r="E86" s="8" t="s">
@@ -22996,14 +22993,14 @@
         <v>15.2</v>
       </c>
       <c r="C87" s="10" t="s">
-        <v>2596</v>
+        <v>2595</v>
       </c>
       <c r="D87" s="10"/>
       <c r="E87" s="8" t="s">
         <v>159</v>
       </c>
       <c r="F87" s="8" t="s">
-        <v>2595</v>
+        <v>2594</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -23011,7 +23008,7 @@
         <v>16</v>
       </c>
       <c r="B88" t="s">
-        <v>2594</v>
+        <v>2593</v>
       </c>
       <c r="C88" s="10"/>
       <c r="D88" s="10"/>
@@ -23024,14 +23021,14 @@
         <v>16.100000000000001</v>
       </c>
       <c r="C89" s="10" t="s">
-        <v>2593</v>
+        <v>2592</v>
       </c>
       <c r="D89" s="10"/>
       <c r="E89" s="8" t="s">
-        <v>2580</v>
+        <v>2579</v>
       </c>
       <c r="F89" s="8" t="s">
-        <v>2592</v>
+        <v>2591</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="30" customHeight="1">
@@ -23042,100 +23039,100 @@
         <v>16.2</v>
       </c>
       <c r="C90" s="10" t="s">
-        <v>2591</v>
+        <v>2590</v>
       </c>
       <c r="D90" s="10"/>
       <c r="E90" s="8" t="s">
-        <v>2580</v>
+        <v>159</v>
       </c>
       <c r="F90" s="8" t="s">
-        <v>2590</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="38.25">
       <c r="A91" t="s">
-        <v>2589</v>
+        <v>2588</v>
       </c>
       <c r="B91" t="s">
-        <v>2589</v>
+        <v>2588</v>
       </c>
       <c r="C91" s="10" t="s">
-        <v>2588</v>
+        <v>2587</v>
       </c>
       <c r="D91" s="10"/>
       <c r="E91" s="8" t="s">
-        <v>2580</v>
+        <v>159</v>
       </c>
       <c r="F91" s="8" t="s">
-        <v>2587</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="A92" t="s">
-        <v>2586</v>
+        <v>2585</v>
       </c>
       <c r="B92" t="s">
-        <v>2586</v>
+        <v>2585</v>
       </c>
       <c r="C92" s="10" t="s">
-        <v>2585</v>
+        <v>2584</v>
       </c>
       <c r="D92" s="10"/>
       <c r="E92" s="8" t="s">
-        <v>2580</v>
+        <v>159</v>
       </c>
     </row>
     <row r="93" spans="1:6">
       <c r="A93" t="s">
-        <v>2584</v>
+        <v>2583</v>
       </c>
       <c r="B93" t="s">
-        <v>2584</v>
+        <v>2583</v>
       </c>
       <c r="C93" s="10" t="s">
-        <v>2583</v>
+        <v>2582</v>
       </c>
       <c r="D93" s="10"/>
       <c r="E93" s="8" t="s">
-        <v>2580</v>
+        <v>159</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c r="A94" t="s">
-        <v>2582</v>
+        <v>2581</v>
       </c>
       <c r="B94" t="s">
-        <v>2582</v>
+        <v>2581</v>
       </c>
       <c r="C94" s="10" t="s">
-        <v>2581</v>
+        <v>2580</v>
       </c>
       <c r="D94" s="10"/>
       <c r="E94" s="8" t="s">
-        <v>2580</v>
+        <v>159</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="25.5">
       <c r="A95" t="s">
-        <v>2579</v>
+        <v>2578</v>
       </c>
       <c r="B95" t="s">
-        <v>2579</v>
+        <v>2578</v>
       </c>
       <c r="C95" s="10" t="s">
-        <v>2578</v>
+        <v>2577</v>
       </c>
       <c r="D95" s="10"/>
     </row>
     <row r="96" spans="1:6">
       <c r="A96" t="s">
-        <v>2577</v>
+        <v>2576</v>
       </c>
       <c r="B96" t="s">
-        <v>2577</v>
+        <v>2576</v>
       </c>
       <c r="C96" s="10" t="s">
-        <v>2576</v>
+        <v>2575</v>
       </c>
       <c r="D96" s="10"/>
     </row>
@@ -23147,11 +23144,11 @@
         <v>16.5</v>
       </c>
       <c r="C97" s="10" t="s">
-        <v>2575</v>
+        <v>2574</v>
       </c>
       <c r="D97" s="10"/>
       <c r="F97" s="8" t="s">
-        <v>2574</v>
+        <v>2573</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="29.45" customHeight="1">
@@ -23162,7 +23159,7 @@
         <v>16.600000000000001</v>
       </c>
       <c r="C98" s="10" t="s">
-        <v>2573</v>
+        <v>2572</v>
       </c>
       <c r="D98" s="10"/>
     </row>
@@ -23174,7 +23171,7 @@
         <v>16.7</v>
       </c>
       <c r="C99" s="10" t="s">
-        <v>2572</v>
+        <v>2571</v>
       </c>
       <c r="D99" s="10"/>
     </row>
@@ -23183,7 +23180,7 @@
         <v>17</v>
       </c>
       <c r="B100" t="s">
-        <v>2571</v>
+        <v>2570</v>
       </c>
       <c r="C100" s="10"/>
       <c r="D100" s="10"/>
@@ -23196,11 +23193,11 @@
         <v>748</v>
       </c>
       <c r="C101" s="10" t="s">
-        <v>2570</v>
+        <v>2569</v>
       </c>
       <c r="D101" s="10"/>
       <c r="E101" s="8" t="s">
-        <v>2792</v>
+        <v>2789</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="25.5">
@@ -23211,11 +23208,11 @@
         <v>749</v>
       </c>
       <c r="C102" s="10" t="s">
-        <v>2569</v>
+        <v>2568</v>
       </c>
       <c r="D102" s="10"/>
       <c r="E102" s="8" t="s">
-        <v>2792</v>
+        <v>2789</v>
       </c>
     </row>
     <row r="103" spans="1:6" ht="38.1" customHeight="1">
@@ -23226,7 +23223,7 @@
         <v>750</v>
       </c>
       <c r="C103" s="10" t="s">
-        <v>2568</v>
+        <v>2567</v>
       </c>
       <c r="D103" s="10"/>
     </row>
@@ -23238,11 +23235,11 @@
         <v>17.2</v>
       </c>
       <c r="C104" s="10" t="s">
-        <v>2567</v>
+        <v>2566</v>
       </c>
       <c r="D104" s="10"/>
       <c r="E104" s="8" t="s">
-        <v>2792</v>
+        <v>2789</v>
       </c>
     </row>
     <row r="105" spans="1:6" ht="60">
@@ -23253,14 +23250,14 @@
         <v>17.3</v>
       </c>
       <c r="C105" s="10" t="s">
-        <v>2566</v>
+        <v>2565</v>
       </c>
       <c r="D105" s="10"/>
       <c r="E105" s="8" t="s">
-        <v>2793</v>
+        <v>2790</v>
       </c>
       <c r="F105" s="8" t="s">
-        <v>2565</v>
+        <v>2564</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -23268,7 +23265,7 @@
         <v>18</v>
       </c>
       <c r="B106" t="s">
-        <v>2564</v>
+        <v>2563</v>
       </c>
       <c r="C106" s="10"/>
       <c r="D106" s="10"/>
@@ -23281,7 +23278,7 @@
         <v>766</v>
       </c>
       <c r="C107" s="10" t="s">
-        <v>2563</v>
+        <v>2562</v>
       </c>
       <c r="D107" s="10"/>
       <c r="E107" s="8" t="s">
@@ -23296,7 +23293,7 @@
         <v>767</v>
       </c>
       <c r="C108" s="10" t="s">
-        <v>2562</v>
+        <v>2561</v>
       </c>
       <c r="D108" s="10"/>
       <c r="E108" s="8" t="s">
@@ -23311,7 +23308,7 @@
         <v>768</v>
       </c>
       <c r="C109" s="10" t="s">
-        <v>2561</v>
+        <v>2560</v>
       </c>
       <c r="D109" s="10"/>
       <c r="E109" s="8" t="s">
@@ -23326,7 +23323,7 @@
         <v>769</v>
       </c>
       <c r="C110" s="10" t="s">
-        <v>2560</v>
+        <v>2559</v>
       </c>
       <c r="D110" s="10"/>
       <c r="E110" s="8" t="s">
@@ -23341,7 +23338,7 @@
         <v>18.2</v>
       </c>
       <c r="C111" s="10" t="s">
-        <v>2559</v>
+        <v>2558</v>
       </c>
       <c r="D111" s="10"/>
       <c r="E111" s="8" t="s">
@@ -23356,7 +23353,7 @@
         <v>18.2</v>
       </c>
       <c r="C112" s="10" t="s">
-        <v>2558</v>
+        <v>2557</v>
       </c>
       <c r="D112" s="10"/>
       <c r="E112" s="8" t="s">
@@ -23371,11 +23368,11 @@
         <v>18.399999999999999</v>
       </c>
       <c r="C113" s="10" t="s">
-        <v>2557</v>
+        <v>2556</v>
       </c>
       <c r="D113" s="10"/>
       <c r="E113" s="8" t="s">
-        <v>2794</v>
+        <v>2791</v>
       </c>
     </row>
     <row r="114" spans="1:6" ht="57.95" customHeight="1">
@@ -23383,96 +23380,96 @@
         <v>19</v>
       </c>
       <c r="B114" t="s">
-        <v>2556</v>
+        <v>2555</v>
       </c>
       <c r="C114" s="10"/>
       <c r="D114" s="10"/>
     </row>
     <row r="115" spans="1:6" ht="42" customHeight="1">
       <c r="A115" t="s">
-        <v>2555</v>
+        <v>2554</v>
       </c>
       <c r="B115" t="s">
-        <v>2555</v>
+        <v>2554</v>
       </c>
       <c r="C115" s="10" t="s">
-        <v>2554</v>
+        <v>2553</v>
       </c>
       <c r="D115" s="10"/>
       <c r="E115" s="8" t="s">
-        <v>2783</v>
+        <v>2780</v>
       </c>
       <c r="F115" s="8" t="s">
-        <v>2553</v>
+        <v>2552</v>
       </c>
     </row>
     <row r="116" spans="1:6">
       <c r="A116" t="s">
-        <v>2552</v>
+        <v>2551</v>
       </c>
       <c r="B116" t="s">
-        <v>2552</v>
+        <v>2551</v>
       </c>
       <c r="C116" s="10" t="s">
-        <v>2551</v>
+        <v>2550</v>
       </c>
       <c r="D116" s="10"/>
     </row>
     <row r="117" spans="1:6">
       <c r="A117" t="s">
-        <v>2550</v>
+        <v>2549</v>
       </c>
       <c r="B117" t="s">
-        <v>2550</v>
+        <v>2549</v>
       </c>
       <c r="C117" s="10" t="s">
-        <v>2549</v>
+        <v>2548</v>
       </c>
       <c r="D117" s="10"/>
     </row>
     <row r="118" spans="1:6" ht="25.5">
       <c r="A118" t="s">
-        <v>2548</v>
+        <v>2547</v>
       </c>
       <c r="B118" t="s">
-        <v>2548</v>
+        <v>2547</v>
       </c>
       <c r="C118" s="10" t="s">
-        <v>2547</v>
+        <v>2546</v>
       </c>
       <c r="D118" s="10"/>
       <c r="E118" s="8" t="s">
-        <v>2783</v>
+        <v>2780</v>
       </c>
     </row>
     <row r="119" spans="1:6" ht="25.5">
       <c r="A119" t="s">
-        <v>2546</v>
+        <v>2545</v>
       </c>
       <c r="B119" t="s">
-        <v>2546</v>
+        <v>2545</v>
       </c>
       <c r="C119" s="10" t="s">
-        <v>2545</v>
+        <v>2544</v>
       </c>
       <c r="D119" s="10"/>
       <c r="E119" s="8" t="s">
-        <v>2783</v>
+        <v>2780</v>
       </c>
     </row>
     <row r="120" spans="1:6" ht="25.5">
       <c r="A120" t="s">
-        <v>2544</v>
+        <v>2543</v>
       </c>
       <c r="B120" t="s">
-        <v>2544</v>
+        <v>2543</v>
       </c>
       <c r="C120" s="10" t="s">
-        <v>2543</v>
+        <v>2542</v>
       </c>
       <c r="D120" s="10"/>
       <c r="E120" s="8" t="s">
-        <v>2783</v>
+        <v>2780</v>
       </c>
     </row>
     <row r="121" spans="1:6">
@@ -23480,38 +23477,38 @@
         <v>20</v>
       </c>
       <c r="B121" t="s">
-        <v>2542</v>
+        <v>2541</v>
       </c>
       <c r="C121" s="10"/>
       <c r="D121" s="10"/>
     </row>
     <row r="122" spans="1:6" ht="47.1" customHeight="1">
       <c r="A122" t="s">
-        <v>2541</v>
+        <v>2540</v>
       </c>
       <c r="B122" t="s">
-        <v>2541</v>
+        <v>2540</v>
       </c>
       <c r="C122" s="10" t="s">
-        <v>2540</v>
+        <v>2539</v>
       </c>
       <c r="D122" s="10"/>
       <c r="E122" s="8" t="s">
-        <v>2784</v>
+        <v>2781</v>
       </c>
       <c r="F122" s="8" t="s">
-        <v>2539</v>
+        <v>2538</v>
       </c>
     </row>
     <row r="123" spans="1:6">
       <c r="A123" t="s">
-        <v>2538</v>
+        <v>2537</v>
       </c>
       <c r="B123" t="s">
-        <v>2538</v>
+        <v>2537</v>
       </c>
       <c r="C123" s="10" t="s">
-        <v>2537</v>
+        <v>2536</v>
       </c>
       <c r="D123" s="10"/>
       <c r="E123" s="8" t="s">
@@ -23520,46 +23517,46 @@
     </row>
     <row r="124" spans="1:6">
       <c r="A124" t="s">
-        <v>2536</v>
+        <v>2535</v>
       </c>
       <c r="B124" t="s">
-        <v>2536</v>
+        <v>2535</v>
       </c>
       <c r="C124" s="10" t="s">
-        <v>2535</v>
+        <v>2534</v>
       </c>
       <c r="D124" s="10"/>
       <c r="E124" s="8" t="s">
-        <v>2785</v>
+        <v>2782</v>
       </c>
     </row>
     <row r="125" spans="1:6" ht="47.1" customHeight="1">
       <c r="A125" t="s">
-        <v>2534</v>
+        <v>2533</v>
       </c>
       <c r="B125" t="s">
-        <v>2534</v>
+        <v>2533</v>
       </c>
       <c r="C125" s="10" t="s">
-        <v>2533</v>
+        <v>2532</v>
       </c>
       <c r="D125" s="10"/>
       <c r="E125" s="8" t="s">
         <v>205</v>
       </c>
       <c r="F125" s="8" t="s">
-        <v>2532</v>
+        <v>2531</v>
       </c>
     </row>
     <row r="126" spans="1:6" ht="38.25">
       <c r="A126" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="B126" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="C126" s="10" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="D126" s="10"/>
       <c r="E126" s="8" t="s">
@@ -23568,31 +23565,31 @@
     </row>
     <row r="127" spans="1:6" ht="45">
       <c r="A127" t="s">
-        <v>2529</v>
+        <v>2528</v>
       </c>
       <c r="B127" t="s">
-        <v>2529</v>
+        <v>2528</v>
       </c>
       <c r="C127" s="10" t="s">
-        <v>2528</v>
+        <v>2527</v>
       </c>
       <c r="D127" s="10"/>
       <c r="E127" s="8" t="s">
         <v>190</v>
       </c>
       <c r="F127" s="8" t="s">
-        <v>2527</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="128" spans="1:6">
       <c r="A128" t="s">
-        <v>2526</v>
+        <v>2525</v>
       </c>
       <c r="B128" t="s">
-        <v>2526</v>
+        <v>2525</v>
       </c>
       <c r="C128" s="10" t="s">
-        <v>2525</v>
+        <v>2524</v>
       </c>
       <c r="D128" s="10"/>
       <c r="E128" s="8" t="s">
@@ -23601,13 +23598,13 @@
     </row>
     <row r="129" spans="1:6">
       <c r="A129" t="s">
-        <v>2524</v>
+        <v>2523</v>
       </c>
       <c r="B129" t="s">
-        <v>2524</v>
+        <v>2523</v>
       </c>
       <c r="C129" s="10" t="s">
-        <v>2523</v>
+        <v>2522</v>
       </c>
       <c r="D129" s="10"/>
       <c r="E129" s="8" t="s">
@@ -23616,13 +23613,13 @@
     </row>
     <row r="130" spans="1:6">
       <c r="A130" t="s">
-        <v>2522</v>
+        <v>2521</v>
       </c>
       <c r="B130" t="s">
-        <v>2522</v>
+        <v>2521</v>
       </c>
       <c r="C130" s="10" t="s">
-        <v>2521</v>
+        <v>2520</v>
       </c>
       <c r="D130" s="10"/>
       <c r="E130" s="8" t="s">
@@ -23631,13 +23628,13 @@
     </row>
     <row r="131" spans="1:6" ht="40.5" customHeight="1">
       <c r="A131" t="s">
-        <v>2520</v>
+        <v>2519</v>
       </c>
       <c r="B131" t="s">
-        <v>2520</v>
+        <v>2519</v>
       </c>
       <c r="C131" s="10" t="s">
-        <v>2519</v>
+        <v>2518</v>
       </c>
       <c r="D131" s="10"/>
       <c r="E131" s="8" t="s">
@@ -23652,7 +23649,7 @@
         <v>20.399999999999999</v>
       </c>
       <c r="C132" s="10" t="s">
-        <v>2518</v>
+        <v>2517</v>
       </c>
       <c r="D132" s="10"/>
     </row>
@@ -23664,7 +23661,7 @@
         <v>20.5</v>
       </c>
       <c r="C133" s="10" t="s">
-        <v>2517</v>
+        <v>2516</v>
       </c>
       <c r="D133" s="10"/>
     </row>
@@ -23673,7 +23670,7 @@
         <v>21</v>
       </c>
       <c r="B134" t="s">
-        <v>2516</v>
+        <v>2515</v>
       </c>
       <c r="C134" s="10"/>
       <c r="D134" s="10"/>
@@ -23686,7 +23683,7 @@
         <v>21.1</v>
       </c>
       <c r="C135" s="10" t="s">
-        <v>2515</v>
+        <v>2514</v>
       </c>
       <c r="D135" s="10"/>
       <c r="E135" s="8" t="s">
@@ -23701,7 +23698,7 @@
         <v>21.2</v>
       </c>
       <c r="C136" s="10" t="s">
-        <v>2514</v>
+        <v>2513</v>
       </c>
       <c r="D136" s="10"/>
       <c r="E136" s="8" t="s">
@@ -23716,7 +23713,7 @@
         <v>21.3</v>
       </c>
       <c r="C137" s="10" t="s">
-        <v>2513</v>
+        <v>2512</v>
       </c>
       <c r="D137" s="10"/>
       <c r="E137" s="8" t="s">
@@ -23731,11 +23728,11 @@
         <v>21.4</v>
       </c>
       <c r="C138" s="10" t="s">
-        <v>2512</v>
+        <v>2511</v>
       </c>
       <c r="D138" s="10"/>
       <c r="E138" s="8" t="s">
-        <v>2511</v>
+        <v>2510</v>
       </c>
     </row>
     <row r="139" spans="1:6" ht="25.5">
@@ -23746,11 +23743,11 @@
         <v>21.5</v>
       </c>
       <c r="C139" s="10" t="s">
-        <v>2510</v>
+        <v>2509</v>
       </c>
       <c r="D139" s="10"/>
       <c r="E139" s="8" t="s">
-        <v>2511</v>
+        <v>2510</v>
       </c>
     </row>
     <row r="140" spans="1:6">
@@ -23758,83 +23755,83 @@
         <v>22</v>
       </c>
       <c r="B140" t="s">
-        <v>2509</v>
+        <v>2508</v>
       </c>
       <c r="C140" s="10"/>
       <c r="D140" s="10"/>
     </row>
     <row r="141" spans="1:6" ht="42.95" customHeight="1">
       <c r="A141" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="B141" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="C141" s="10" t="s">
-        <v>2507</v>
+        <v>2506</v>
       </c>
       <c r="D141" s="10"/>
       <c r="E141" s="8" t="s">
-        <v>2795</v>
+        <v>2792</v>
       </c>
       <c r="F141" s="8" t="s">
-        <v>2506</v>
+        <v>2505</v>
       </c>
     </row>
     <row r="142" spans="1:6">
       <c r="A142" t="s">
-        <v>2505</v>
+        <v>2504</v>
       </c>
       <c r="B142" t="s">
-        <v>2505</v>
+        <v>2504</v>
       </c>
       <c r="C142" s="10" t="s">
-        <v>2504</v>
+        <v>2503</v>
       </c>
       <c r="D142" s="10"/>
       <c r="E142" s="8" t="s">
-        <v>2753</v>
+        <v>2752</v>
       </c>
     </row>
     <row r="143" spans="1:6" ht="30">
       <c r="A143" t="s">
-        <v>2503</v>
+        <v>2502</v>
       </c>
       <c r="B143" t="s">
-        <v>2503</v>
+        <v>2502</v>
       </c>
       <c r="C143" s="10" t="s">
-        <v>2502</v>
+        <v>2501</v>
       </c>
       <c r="D143" s="10"/>
       <c r="E143" s="8" t="s">
-        <v>2754</v>
+        <v>2753</v>
       </c>
     </row>
     <row r="144" spans="1:6">
       <c r="A144" t="s">
-        <v>2501</v>
+        <v>2500</v>
       </c>
       <c r="B144" t="s">
-        <v>2501</v>
+        <v>2500</v>
       </c>
       <c r="C144" s="10" t="s">
-        <v>2500</v>
+        <v>2499</v>
       </c>
       <c r="D144" s="10"/>
       <c r="E144" s="8" t="s">
-        <v>2755</v>
+        <v>2754</v>
       </c>
     </row>
     <row r="145" spans="1:6">
       <c r="A145" t="s">
-        <v>2499</v>
+        <v>2498</v>
       </c>
       <c r="B145" t="s">
-        <v>2499</v>
+        <v>2498</v>
       </c>
       <c r="C145" s="10" t="s">
-        <v>2498</v>
+        <v>2497</v>
       </c>
       <c r="D145" s="10"/>
       <c r="E145" s="8">
@@ -23843,28 +23840,28 @@
     </row>
     <row r="146" spans="1:6">
       <c r="A146" t="s">
-        <v>2497</v>
+        <v>2496</v>
       </c>
       <c r="B146" t="s">
-        <v>2497</v>
+        <v>2496</v>
       </c>
       <c r="C146" s="10" t="s">
-        <v>2496</v>
+        <v>2495</v>
       </c>
       <c r="D146" s="10"/>
       <c r="E146" s="8" t="s">
-        <v>2796</v>
+        <v>2805</v>
       </c>
     </row>
     <row r="147" spans="1:6">
       <c r="A147" t="s">
-        <v>2495</v>
+        <v>2494</v>
       </c>
       <c r="B147" t="s">
-        <v>2495</v>
+        <v>2494</v>
       </c>
       <c r="C147" s="10" t="s">
-        <v>2494</v>
+        <v>2493</v>
       </c>
       <c r="D147" s="10"/>
       <c r="E147" s="8">
@@ -23879,7 +23876,7 @@
         <v>22.2</v>
       </c>
       <c r="C148" s="10" t="s">
-        <v>2493</v>
+        <v>2492</v>
       </c>
       <c r="D148" s="10"/>
     </row>
@@ -23891,7 +23888,7 @@
         <v>22.3</v>
       </c>
       <c r="C149" s="10" t="s">
-        <v>2492</v>
+        <v>2491</v>
       </c>
       <c r="D149" s="10"/>
     </row>
@@ -23903,7 +23900,7 @@
         <v>22.4</v>
       </c>
       <c r="C150" s="10" t="s">
-        <v>2491</v>
+        <v>2490</v>
       </c>
       <c r="D150" s="10"/>
     </row>
@@ -23912,38 +23909,38 @@
         <v>23</v>
       </c>
       <c r="B151" t="s">
-        <v>2490</v>
+        <v>2489</v>
       </c>
       <c r="C151" s="10"/>
       <c r="D151" s="10"/>
     </row>
     <row r="152" spans="1:6" ht="48" customHeight="1">
       <c r="A152" t="s">
-        <v>2489</v>
+        <v>2488</v>
       </c>
       <c r="B152" t="s">
-        <v>2489</v>
+        <v>2488</v>
       </c>
       <c r="C152" s="10" t="s">
-        <v>2488</v>
+        <v>2487</v>
       </c>
       <c r="D152" s="10"/>
       <c r="E152" s="8" t="s">
         <v>673</v>
       </c>
       <c r="F152" s="8" t="s">
-        <v>2487</v>
+        <v>2486</v>
       </c>
     </row>
     <row r="153" spans="1:6">
       <c r="A153" t="s">
-        <v>2486</v>
+        <v>2485</v>
       </c>
       <c r="B153" t="s">
-        <v>2486</v>
+        <v>2485</v>
       </c>
       <c r="C153" s="10" t="s">
-        <v>2485</v>
+        <v>2484</v>
       </c>
       <c r="D153" s="10"/>
       <c r="E153" s="8" t="s">
@@ -23952,46 +23949,46 @@
     </row>
     <row r="154" spans="1:6" ht="26.45" customHeight="1">
       <c r="A154" t="s">
-        <v>2484</v>
+        <v>2483</v>
       </c>
       <c r="B154" t="s">
-        <v>2484</v>
+        <v>2483</v>
       </c>
       <c r="C154" s="10" t="s">
-        <v>2483</v>
+        <v>2482</v>
       </c>
       <c r="D154" s="10"/>
       <c r="E154" s="8" t="s">
-        <v>2756</v>
+        <v>2755</v>
       </c>
     </row>
     <row r="155" spans="1:6" ht="25.5">
       <c r="A155" t="s">
-        <v>2482</v>
+        <v>2481</v>
       </c>
       <c r="B155" t="s">
-        <v>2482</v>
+        <v>2481</v>
       </c>
       <c r="C155" s="10" t="s">
-        <v>2481</v>
+        <v>2480</v>
       </c>
       <c r="D155" s="10"/>
       <c r="E155" s="8" t="s">
         <v>673</v>
       </c>
       <c r="F155" s="8" t="s">
-        <v>2480</v>
+        <v>2479</v>
       </c>
     </row>
     <row r="156" spans="1:6">
       <c r="A156" t="s">
-        <v>2479</v>
+        <v>2478</v>
       </c>
       <c r="B156" t="s">
-        <v>2479</v>
+        <v>2478</v>
       </c>
       <c r="C156" s="10" t="s">
-        <v>2478</v>
+        <v>2477</v>
       </c>
       <c r="D156" s="10"/>
       <c r="E156" s="8" t="s">
@@ -24000,28 +23997,28 @@
     </row>
     <row r="157" spans="1:6" ht="25.5">
       <c r="A157" t="s">
-        <v>2477</v>
+        <v>2476</v>
       </c>
       <c r="B157" t="s">
-        <v>2477</v>
+        <v>2476</v>
       </c>
       <c r="C157" s="10" t="s">
-        <v>2476</v>
+        <v>2475</v>
       </c>
       <c r="D157" s="10"/>
       <c r="F157" s="8" t="s">
-        <v>2475</v>
+        <v>2474</v>
       </c>
     </row>
     <row r="158" spans="1:6" ht="25.5">
       <c r="A158" t="s">
-        <v>2474</v>
+        <v>2473</v>
       </c>
       <c r="B158" t="s">
-        <v>2474</v>
+        <v>2473</v>
       </c>
       <c r="C158" s="10" t="s">
-        <v>2473</v>
+        <v>2472</v>
       </c>
       <c r="D158" s="10"/>
       <c r="E158" s="8" t="s">
@@ -24030,13 +24027,13 @@
     </row>
     <row r="159" spans="1:6">
       <c r="A159" t="s">
-        <v>2472</v>
+        <v>2471</v>
       </c>
       <c r="B159" t="s">
-        <v>2472</v>
+        <v>2471</v>
       </c>
       <c r="C159" s="10" t="s">
-        <v>2471</v>
+        <v>2470</v>
       </c>
       <c r="D159" s="10"/>
       <c r="E159" s="8" t="s">
@@ -24051,7 +24048,7 @@
         <v>23.2</v>
       </c>
       <c r="C160" s="10" t="s">
-        <v>2470</v>
+        <v>2469</v>
       </c>
       <c r="D160" s="10"/>
       <c r="E160" s="8" t="s">
@@ -24066,11 +24063,11 @@
         <v>23.3</v>
       </c>
       <c r="C161" s="10" t="s">
-        <v>2469</v>
+        <v>2468</v>
       </c>
       <c r="D161" s="10"/>
       <c r="E161" s="8" t="s">
-        <v>2757</v>
+        <v>2756</v>
       </c>
     </row>
     <row r="162" spans="1:6" ht="25.5">
@@ -24081,7 +24078,7 @@
         <v>23.4</v>
       </c>
       <c r="C162" s="10" t="s">
-        <v>2468</v>
+        <v>2467</v>
       </c>
       <c r="D162" s="10"/>
       <c r="E162" s="8" t="s">
@@ -24096,7 +24093,7 @@
         <v>23.5</v>
       </c>
       <c r="C163" s="10" t="s">
-        <v>2467</v>
+        <v>2466</v>
       </c>
       <c r="D163" s="10"/>
     </row>
@@ -24105,35 +24102,35 @@
         <v>24</v>
       </c>
       <c r="B164" t="s">
-        <v>2466</v>
+        <v>2465</v>
       </c>
       <c r="C164" s="10"/>
       <c r="D164" s="10"/>
     </row>
     <row r="165" spans="1:6" ht="60" customHeight="1">
       <c r="A165" t="s">
-        <v>2465</v>
+        <v>2464</v>
       </c>
       <c r="B165" t="s">
-        <v>2465</v>
+        <v>2464</v>
       </c>
       <c r="C165" s="10" t="s">
-        <v>2464</v>
+        <v>2463</v>
       </c>
       <c r="D165" s="10"/>
       <c r="E165" s="8" t="s">
-        <v>2758</v>
+        <v>2757</v>
       </c>
     </row>
     <row r="166" spans="1:6">
       <c r="A166" t="s">
-        <v>2463</v>
+        <v>2462</v>
       </c>
       <c r="B166" t="s">
-        <v>2463</v>
+        <v>2462</v>
       </c>
       <c r="C166" s="10" t="s">
-        <v>2462</v>
+        <v>2461</v>
       </c>
       <c r="D166" s="10"/>
       <c r="E166" s="8" t="s">
@@ -24142,13 +24139,13 @@
     </row>
     <row r="167" spans="1:6">
       <c r="A167" t="s">
-        <v>2461</v>
+        <v>2460</v>
       </c>
       <c r="B167" t="s">
-        <v>2461</v>
+        <v>2460</v>
       </c>
       <c r="C167" s="10" t="s">
-        <v>2460</v>
+        <v>2459</v>
       </c>
       <c r="D167" s="10"/>
       <c r="E167" s="8" t="s">
@@ -24163,11 +24160,11 @@
         <v>24.2</v>
       </c>
       <c r="C168" s="10" t="s">
-        <v>2459</v>
+        <v>2458</v>
       </c>
       <c r="D168" s="10"/>
       <c r="E168" s="8" t="s">
-        <v>2759</v>
+        <v>2758</v>
       </c>
     </row>
     <row r="169" spans="1:6" ht="90">
@@ -24175,7 +24172,7 @@
         <v>25</v>
       </c>
       <c r="B169" s="9" t="s">
-        <v>2458</v>
+        <v>2457</v>
       </c>
       <c r="C169" s="10"/>
       <c r="D169" s="10"/>
@@ -24188,25 +24185,25 @@
         <v>25.1</v>
       </c>
       <c r="C170" s="10" t="s">
-        <v>2457</v>
+        <v>2456</v>
       </c>
       <c r="D170" s="10"/>
       <c r="E170" s="8" t="s">
         <v>887</v>
       </c>
       <c r="F170" s="8" t="s">
-        <v>2456</v>
+        <v>2455</v>
       </c>
     </row>
     <row r="171" spans="1:6" ht="25.5">
       <c r="A171" t="s">
-        <v>2455</v>
+        <v>2454</v>
       </c>
       <c r="B171" t="s">
-        <v>2455</v>
+        <v>2454</v>
       </c>
       <c r="C171" s="10" t="s">
-        <v>2454</v>
+        <v>2453</v>
       </c>
       <c r="D171" s="10"/>
       <c r="E171" s="8" t="s">
@@ -24215,13 +24212,13 @@
     </row>
     <row r="172" spans="1:6">
       <c r="A172" t="s">
-        <v>2453</v>
+        <v>2452</v>
       </c>
       <c r="B172" t="s">
-        <v>2453</v>
+        <v>2452</v>
       </c>
       <c r="C172" s="10" t="s">
-        <v>2452</v>
+        <v>2451</v>
       </c>
       <c r="D172" s="10"/>
       <c r="E172" s="8" t="s">
@@ -24230,13 +24227,13 @@
     </row>
     <row r="173" spans="1:6">
       <c r="A173" t="s">
-        <v>2451</v>
+        <v>2450</v>
       </c>
       <c r="B173" t="s">
-        <v>2451</v>
+        <v>2450</v>
       </c>
       <c r="C173" s="10" t="s">
-        <v>2450</v>
+        <v>2449</v>
       </c>
       <c r="D173" s="10"/>
       <c r="E173" s="8" t="s">
@@ -24245,13 +24242,13 @@
     </row>
     <row r="174" spans="1:6">
       <c r="A174" t="s">
-        <v>2449</v>
+        <v>2448</v>
       </c>
       <c r="B174" t="s">
-        <v>2449</v>
+        <v>2448</v>
       </c>
       <c r="C174" s="10" t="s">
-        <v>2448</v>
+        <v>2447</v>
       </c>
       <c r="D174" s="10"/>
       <c r="E174" s="8" t="s">
@@ -24266,14 +24263,14 @@
         <v>25.3</v>
       </c>
       <c r="C175" s="10" t="s">
-        <v>2447</v>
+        <v>2446</v>
       </c>
       <c r="D175" s="10"/>
       <c r="E175" s="8" t="s">
         <v>887</v>
       </c>
       <c r="F175" s="8" t="s">
-        <v>2446</v>
+        <v>2445</v>
       </c>
     </row>
     <row r="176" spans="1:6" ht="25.5">
@@ -24284,7 +24281,7 @@
         <v>25.4</v>
       </c>
       <c r="C176" s="10" t="s">
-        <v>2445</v>
+        <v>2444</v>
       </c>
       <c r="D176" s="10"/>
       <c r="E176" s="8" t="s">
@@ -24299,11 +24296,11 @@
         <v>25.5</v>
       </c>
       <c r="C177" s="10" t="s">
-        <v>2444</v>
+        <v>2443</v>
       </c>
       <c r="D177" s="10"/>
       <c r="F177" s="8" t="s">
-        <v>2443</v>
+        <v>2442</v>
       </c>
     </row>
     <row r="178" spans="1:6" ht="39.950000000000003" customHeight="1">
@@ -24314,7 +24311,7 @@
         <v>25.6</v>
       </c>
       <c r="C178" s="10" t="s">
-        <v>2442</v>
+        <v>2441</v>
       </c>
       <c r="D178" s="10"/>
     </row>
@@ -24326,7 +24323,7 @@
         <v>25.7</v>
       </c>
       <c r="C179" s="10" t="s">
-        <v>2441</v>
+        <v>2440</v>
       </c>
       <c r="D179" s="10"/>
     </row>
@@ -24335,102 +24332,102 @@
         <v>26</v>
       </c>
       <c r="B180" t="s">
-        <v>2440</v>
+        <v>2439</v>
       </c>
       <c r="C180" s="10"/>
       <c r="D180" s="10"/>
     </row>
     <row r="181" spans="1:6" ht="40.5" customHeight="1">
       <c r="A181" t="s">
-        <v>2439</v>
+        <v>2438</v>
       </c>
       <c r="B181" t="s">
-        <v>2439</v>
+        <v>2438</v>
       </c>
       <c r="C181" s="10" t="s">
-        <v>2438</v>
+        <v>2437</v>
       </c>
       <c r="D181" s="10"/>
       <c r="E181" s="8" t="s">
-        <v>2798</v>
+        <v>2794</v>
       </c>
       <c r="F181" s="8" t="s">
-        <v>2437</v>
+        <v>2436</v>
       </c>
     </row>
     <row r="182" spans="1:6">
       <c r="A182" t="s">
-        <v>2436</v>
+        <v>2435</v>
       </c>
       <c r="B182" t="s">
-        <v>2436</v>
+        <v>2435</v>
       </c>
       <c r="C182" s="10" t="s">
-        <v>2435</v>
+        <v>2434</v>
       </c>
       <c r="D182" s="10"/>
       <c r="E182" s="8" t="s">
-        <v>2798</v>
+        <v>2794</v>
       </c>
     </row>
     <row r="183" spans="1:6">
       <c r="A183" t="s">
-        <v>2434</v>
+        <v>2433</v>
       </c>
       <c r="B183" t="s">
-        <v>2434</v>
+        <v>2433</v>
       </c>
       <c r="C183" s="10" t="s">
-        <v>2433</v>
+        <v>2432</v>
       </c>
       <c r="D183" s="10"/>
       <c r="E183" s="8" t="s">
-        <v>2798</v>
+        <v>2794</v>
       </c>
     </row>
     <row r="184" spans="1:6">
       <c r="A184" t="s">
-        <v>2432</v>
+        <v>2431</v>
       </c>
       <c r="B184" t="s">
-        <v>2432</v>
+        <v>2431</v>
       </c>
       <c r="C184" s="10" t="s">
-        <v>2431</v>
+        <v>2430</v>
       </c>
       <c r="D184" s="10"/>
       <c r="E184" s="8" t="s">
-        <v>2798</v>
+        <v>2794</v>
       </c>
     </row>
     <row r="185" spans="1:6">
       <c r="A185" t="s">
-        <v>2430</v>
+        <v>2429</v>
       </c>
       <c r="B185" t="s">
-        <v>2430</v>
+        <v>2429</v>
       </c>
       <c r="C185" s="10" t="s">
-        <v>2429</v>
+        <v>2428</v>
       </c>
       <c r="D185" s="10"/>
       <c r="E185" s="8" t="s">
-        <v>2798</v>
+        <v>2794</v>
       </c>
     </row>
     <row r="186" spans="1:6">
       <c r="A186" t="s">
-        <v>2428</v>
+        <v>2427</v>
       </c>
       <c r="B186" t="s">
-        <v>2428</v>
+        <v>2427</v>
       </c>
       <c r="C186" s="10" t="s">
-        <v>2427</v>
+        <v>2426</v>
       </c>
       <c r="D186" s="10"/>
       <c r="E186" s="8" t="s">
-        <v>2798</v>
+        <v>2794</v>
       </c>
     </row>
     <row r="187" spans="1:6" ht="26.45" customHeight="1">
@@ -24441,11 +24438,11 @@
         <v>26.2</v>
       </c>
       <c r="C187" s="10" t="s">
-        <v>2426</v>
+        <v>2425</v>
       </c>
       <c r="D187" s="10"/>
       <c r="E187" s="8" t="s">
-        <v>2760</v>
+        <v>2759</v>
       </c>
     </row>
     <row r="188" spans="1:6" ht="41.45" customHeight="1">
@@ -24456,7 +24453,7 @@
         <v>26.3</v>
       </c>
       <c r="C188" s="10" t="s">
-        <v>2425</v>
+        <v>2424</v>
       </c>
       <c r="D188" s="10"/>
     </row>
@@ -24468,7 +24465,7 @@
         <v>26.4</v>
       </c>
       <c r="C189" s="10" t="s">
-        <v>2424</v>
+        <v>2423</v>
       </c>
       <c r="D189" s="10"/>
     </row>
@@ -24477,7 +24474,7 @@
         <v>27</v>
       </c>
       <c r="B190" s="9" t="s">
-        <v>2423</v>
+        <v>2422</v>
       </c>
       <c r="C190" s="10"/>
       <c r="D190" s="10"/>
@@ -24490,7 +24487,7 @@
         <v>27.1</v>
       </c>
       <c r="C191" s="10" t="s">
-        <v>2422</v>
+        <v>2421</v>
       </c>
       <c r="D191" s="10"/>
       <c r="E191" s="8" t="s">
@@ -24505,7 +24502,7 @@
         <v>27.2</v>
       </c>
       <c r="C192" s="10" t="s">
-        <v>2421</v>
+        <v>2420</v>
       </c>
       <c r="D192" s="10"/>
       <c r="E192" s="8" t="s">
@@ -24514,13 +24511,13 @@
     </row>
     <row r="193" spans="1:6" ht="38.25">
       <c r="A193" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
       <c r="B193" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
       <c r="C193" s="10" t="s">
-        <v>2419</v>
+        <v>2418</v>
       </c>
       <c r="D193" s="10"/>
       <c r="E193" s="8" t="s">
@@ -24529,13 +24526,13 @@
     </row>
     <row r="194" spans="1:6" ht="25.5">
       <c r="A194" t="s">
-        <v>2418</v>
+        <v>2417</v>
       </c>
       <c r="B194" t="s">
-        <v>2418</v>
+        <v>2417</v>
       </c>
       <c r="C194" s="10" t="s">
-        <v>2417</v>
+        <v>2416</v>
       </c>
       <c r="D194" s="10"/>
       <c r="E194" s="8" t="s">
@@ -24544,13 +24541,13 @@
     </row>
     <row r="195" spans="1:6">
       <c r="A195" t="s">
-        <v>2416</v>
+        <v>2415</v>
       </c>
       <c r="B195" t="s">
-        <v>2416</v>
+        <v>2415</v>
       </c>
       <c r="C195" s="10" t="s">
-        <v>2415</v>
+        <v>2414</v>
       </c>
       <c r="D195" s="10"/>
       <c r="E195" s="8" t="s">
@@ -24565,14 +24562,14 @@
         <v>27.4</v>
       </c>
       <c r="C196" s="10" t="s">
-        <v>2414</v>
+        <v>2413</v>
       </c>
       <c r="D196" s="10"/>
       <c r="E196" s="8" t="s">
-        <v>2786</v>
+        <v>2783</v>
       </c>
       <c r="F196" s="8" t="s">
-        <v>2413</v>
+        <v>2412</v>
       </c>
     </row>
     <row r="197" spans="1:6" ht="44.45" customHeight="1">
@@ -24583,11 +24580,11 @@
         <v>27.5</v>
       </c>
       <c r="C197" s="10" t="s">
-        <v>2412</v>
+        <v>2411</v>
       </c>
       <c r="D197" s="10"/>
       <c r="E197" s="8" t="s">
-        <v>2786</v>
+        <v>2783</v>
       </c>
     </row>
     <row r="198" spans="1:6" ht="44.45" customHeight="1">
@@ -24595,53 +24592,53 @@
         <v>28</v>
       </c>
       <c r="B198" t="s">
-        <v>2411</v>
+        <v>2410</v>
       </c>
       <c r="C198" s="10"/>
       <c r="D198" s="10"/>
     </row>
     <row r="199" spans="1:6" ht="56.1" customHeight="1">
       <c r="A199" t="s">
-        <v>2410</v>
+        <v>2409</v>
       </c>
       <c r="B199" t="s">
-        <v>2410</v>
+        <v>2409</v>
       </c>
       <c r="C199" s="10" t="s">
-        <v>2409</v>
+        <v>2408</v>
       </c>
       <c r="D199" s="10"/>
       <c r="E199" s="8" t="s">
-        <v>2799</v>
+        <v>2795</v>
       </c>
       <c r="F199" s="8" t="s">
-        <v>2408</v>
+        <v>2407</v>
       </c>
     </row>
     <row r="200" spans="1:6">
       <c r="A200" t="s">
-        <v>2407</v>
+        <v>2406</v>
       </c>
       <c r="B200" t="s">
-        <v>2407</v>
+        <v>2406</v>
       </c>
       <c r="C200" s="10" t="s">
-        <v>2406</v>
+        <v>2405</v>
       </c>
       <c r="D200" s="10"/>
       <c r="E200" s="8" t="s">
-        <v>2761</v>
+        <v>2760</v>
       </c>
     </row>
     <row r="201" spans="1:6">
       <c r="A201" t="s">
-        <v>2405</v>
+        <v>2404</v>
       </c>
       <c r="B201" t="s">
-        <v>2405</v>
+        <v>2404</v>
       </c>
       <c r="C201" s="10" t="s">
-        <v>2404</v>
+        <v>2403</v>
       </c>
       <c r="D201" s="10"/>
       <c r="E201" s="8" t="s">
@@ -24650,13 +24647,13 @@
     </row>
     <row r="202" spans="1:6">
       <c r="A202" t="s">
-        <v>2403</v>
+        <v>2402</v>
       </c>
       <c r="B202" t="s">
-        <v>2403</v>
+        <v>2402</v>
       </c>
       <c r="C202" s="10" t="s">
-        <v>2402</v>
+        <v>2401</v>
       </c>
       <c r="D202" s="10"/>
     </row>
@@ -24668,7 +24665,7 @@
         <v>28.2</v>
       </c>
       <c r="C203" s="10" t="s">
-        <v>2401</v>
+        <v>2400</v>
       </c>
       <c r="D203" s="10"/>
     </row>
@@ -24680,11 +24677,11 @@
         <v>28.3</v>
       </c>
       <c r="C204" s="10" t="s">
-        <v>2400</v>
+        <v>2399</v>
       </c>
       <c r="D204" s="10"/>
       <c r="F204" s="8" t="s">
-        <v>2399</v>
+        <v>2398</v>
       </c>
     </row>
     <row r="205" spans="1:6" ht="25.5">
@@ -24695,7 +24692,7 @@
         <v>28.4</v>
       </c>
       <c r="C205" s="10" t="s">
-        <v>2398</v>
+        <v>2397</v>
       </c>
       <c r="D205" s="10"/>
     </row>
@@ -24704,7 +24701,7 @@
         <v>29</v>
       </c>
       <c r="B206" t="s">
-        <v>2397</v>
+        <v>2396</v>
       </c>
       <c r="C206" s="10"/>
       <c r="D206" s="10"/>
@@ -24717,97 +24714,97 @@
         <v>29.1</v>
       </c>
       <c r="C207" s="10" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="D207" s="10"/>
       <c r="E207" s="8" t="s">
-        <v>2762</v>
+        <v>2761</v>
       </c>
       <c r="F207" s="8" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
     </row>
     <row r="208" spans="1:6" ht="27.6" customHeight="1">
       <c r="A208" t="s">
-        <v>2394</v>
+        <v>2393</v>
       </c>
       <c r="B208" t="s">
-        <v>2394</v>
+        <v>2393</v>
       </c>
       <c r="C208" s="10" t="s">
-        <v>2393</v>
+        <v>2392</v>
       </c>
       <c r="D208" s="10"/>
     </row>
     <row r="209" spans="1:5">
       <c r="A209" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="B209" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="C209" s="10" t="s">
-        <v>2391</v>
+        <v>2390</v>
       </c>
       <c r="D209" s="10"/>
     </row>
     <row r="210" spans="1:5">
       <c r="A210" t="s">
-        <v>2390</v>
+        <v>2389</v>
       </c>
       <c r="B210" t="s">
-        <v>2390</v>
+        <v>2389</v>
       </c>
       <c r="C210" s="10" t="s">
-        <v>2389</v>
+        <v>2388</v>
       </c>
       <c r="D210" s="10"/>
     </row>
     <row r="211" spans="1:5">
       <c r="A211" t="s">
-        <v>2388</v>
+        <v>2387</v>
       </c>
       <c r="B211" t="s">
-        <v>2388</v>
+        <v>2387</v>
       </c>
       <c r="C211" s="10" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
       <c r="D211" s="10"/>
     </row>
     <row r="212" spans="1:5" ht="25.5">
       <c r="A212" t="s">
-        <v>2386</v>
+        <v>2385</v>
       </c>
       <c r="B212" t="s">
-        <v>2386</v>
+        <v>2385</v>
       </c>
       <c r="C212" s="10" t="s">
-        <v>2385</v>
+        <v>2384</v>
       </c>
       <c r="D212" s="10"/>
     </row>
     <row r="213" spans="1:5">
       <c r="A213" t="s">
-        <v>2384</v>
+        <v>2383</v>
       </c>
       <c r="B213" t="s">
-        <v>2384</v>
+        <v>2383</v>
       </c>
       <c r="C213" s="10" t="s">
-        <v>2383</v>
+        <v>2382</v>
       </c>
       <c r="D213" s="10"/>
     </row>
     <row r="214" spans="1:5">
       <c r="A214" t="s">
-        <v>2382</v>
+        <v>2381</v>
       </c>
       <c r="B214" t="s">
-        <v>2382</v>
+        <v>2381</v>
       </c>
       <c r="C214" s="10" t="s">
-        <v>2381</v>
+        <v>2380</v>
       </c>
       <c r="D214" s="10"/>
     </row>
@@ -24819,7 +24816,7 @@
         <v>29.3</v>
       </c>
       <c r="C215" s="10" t="s">
-        <v>2380</v>
+        <v>2379</v>
       </c>
       <c r="D215" s="10"/>
     </row>
@@ -24831,7 +24828,7 @@
         <v>29.4</v>
       </c>
       <c r="C216" s="10" t="s">
-        <v>2379</v>
+        <v>2378</v>
       </c>
       <c r="D216" s="10"/>
     </row>
@@ -24843,7 +24840,7 @@
         <v>29.5</v>
       </c>
       <c r="C217" s="10" t="s">
-        <v>2378</v>
+        <v>2377</v>
       </c>
       <c r="D217" s="10"/>
     </row>
@@ -24855,7 +24852,7 @@
         <v>29.6</v>
       </c>
       <c r="C218" s="10" t="s">
-        <v>2377</v>
+        <v>2376</v>
       </c>
       <c r="D218" s="10"/>
     </row>
@@ -24867,7 +24864,7 @@
         <v>29.7</v>
       </c>
       <c r="C219" s="10" t="s">
-        <v>2376</v>
+        <v>2375</v>
       </c>
       <c r="D219" s="10"/>
     </row>
@@ -24876,7 +24873,7 @@
         <v>30</v>
       </c>
       <c r="B220" t="s">
-        <v>2375</v>
+        <v>2374</v>
       </c>
       <c r="C220" s="10"/>
       <c r="D220" s="10"/>
@@ -24889,7 +24886,7 @@
         <v>850</v>
       </c>
       <c r="C221" s="10" t="s">
-        <v>2374</v>
+        <v>2373</v>
       </c>
       <c r="D221" s="10"/>
       <c r="E221" s="8" t="s">
@@ -24904,7 +24901,7 @@
         <v>851</v>
       </c>
       <c r="C222" s="10" t="s">
-        <v>2373</v>
+        <v>2372</v>
       </c>
       <c r="D222" s="10"/>
       <c r="E222" s="8" t="s">
@@ -24919,11 +24916,11 @@
         <v>852</v>
       </c>
       <c r="C223" s="10" t="s">
-        <v>2372</v>
+        <v>2371</v>
       </c>
       <c r="D223" s="10"/>
       <c r="E223" s="8" t="s">
-        <v>2787</v>
+        <v>2784</v>
       </c>
     </row>
     <row r="224" spans="1:5" ht="25.5">
@@ -24934,7 +24931,7 @@
         <v>853</v>
       </c>
       <c r="C224" s="10" t="s">
-        <v>2371</v>
+        <v>2370</v>
       </c>
       <c r="D224" s="10"/>
       <c r="E224" s="8" t="s">
@@ -24949,7 +24946,7 @@
         <v>855</v>
       </c>
       <c r="C225" s="10" t="s">
-        <v>2370</v>
+        <v>2369</v>
       </c>
       <c r="D225" s="10"/>
       <c r="E225" s="8" t="s">
@@ -24964,7 +24961,7 @@
         <v>857</v>
       </c>
       <c r="C226" s="10" t="s">
-        <v>2369</v>
+        <v>2368</v>
       </c>
       <c r="D226" s="10"/>
       <c r="E226" s="8" t="s">
@@ -24979,7 +24976,7 @@
         <v>859</v>
       </c>
       <c r="C227" s="10" t="s">
-        <v>2368</v>
+        <v>2367</v>
       </c>
       <c r="D227" s="10"/>
       <c r="E227" s="8" t="s">
@@ -24994,7 +24991,7 @@
         <v>30.2</v>
       </c>
       <c r="C228" s="10" t="s">
-        <v>2367</v>
+        <v>2366</v>
       </c>
       <c r="D228" s="10"/>
     </row>
@@ -25006,14 +25003,14 @@
         <v>30.3</v>
       </c>
       <c r="C229" s="10" t="s">
-        <v>2366</v>
+        <v>2365</v>
       </c>
       <c r="D229" s="10"/>
       <c r="E229" s="8" t="s">
         <v>33</v>
       </c>
       <c r="F229" s="8" t="s">
-        <v>2365</v>
+        <v>2364</v>
       </c>
     </row>
     <row r="230" spans="1:6">
@@ -25021,7 +25018,7 @@
         <v>31</v>
       </c>
       <c r="B230" t="s">
-        <v>2364</v>
+        <v>2363</v>
       </c>
       <c r="C230" s="10"/>
       <c r="D230" s="10"/>
@@ -25034,14 +25031,14 @@
         <v>31.1</v>
       </c>
       <c r="C231" s="10" t="s">
-        <v>2363</v>
+        <v>2362</v>
       </c>
       <c r="D231" s="10"/>
       <c r="E231" s="8" t="s">
-        <v>2800</v>
+        <v>2796</v>
       </c>
       <c r="F231" s="8" t="s">
-        <v>2362</v>
+        <v>2361</v>
       </c>
     </row>
     <row r="232" spans="1:6" ht="45">
@@ -25052,14 +25049,14 @@
         <v>31.2</v>
       </c>
       <c r="C232" s="10" t="s">
-        <v>2361</v>
+        <v>2360</v>
       </c>
       <c r="D232" s="10"/>
       <c r="E232" s="8" t="s">
         <v>824</v>
       </c>
       <c r="F232" s="8" t="s">
-        <v>2360</v>
+        <v>2359</v>
       </c>
     </row>
     <row r="233" spans="1:6" ht="35.1" customHeight="1">
@@ -25070,11 +25067,11 @@
         <v>31.3</v>
       </c>
       <c r="C233" s="10" t="s">
-        <v>2359</v>
+        <v>2358</v>
       </c>
       <c r="D233" s="10"/>
       <c r="E233" s="8" t="s">
-        <v>2763</v>
+        <v>2762</v>
       </c>
     </row>
     <row r="234" spans="1:6" ht="35.1" customHeight="1">
@@ -25082,7 +25079,7 @@
         <v>32</v>
       </c>
       <c r="B234" t="s">
-        <v>2358</v>
+        <v>2357</v>
       </c>
       <c r="C234" s="10"/>
       <c r="D234" s="10"/>
@@ -25095,41 +25092,41 @@
         <v>32.1</v>
       </c>
       <c r="C235" s="10" t="s">
-        <v>2357</v>
+        <v>2356</v>
       </c>
       <c r="D235" s="10"/>
       <c r="E235" s="8" t="s">
-        <v>2801</v>
+        <v>2797</v>
       </c>
     </row>
     <row r="236" spans="1:6" ht="38.25">
       <c r="A236" t="s">
-        <v>2356</v>
+        <v>2355</v>
       </c>
       <c r="B236" t="s">
-        <v>2356</v>
+        <v>2355</v>
       </c>
       <c r="C236" s="10" t="s">
-        <v>2355</v>
+        <v>2354</v>
       </c>
       <c r="D236" s="10"/>
       <c r="E236" s="8" t="s">
-        <v>2801</v>
+        <v>2797</v>
       </c>
     </row>
     <row r="237" spans="1:6">
       <c r="A237" t="s">
-        <v>2354</v>
+        <v>2353</v>
       </c>
       <c r="B237" t="s">
-        <v>2354</v>
+        <v>2353</v>
       </c>
       <c r="C237" s="10" t="s">
-        <v>2353</v>
+        <v>2352</v>
       </c>
       <c r="D237" s="10"/>
       <c r="E237" s="8" t="s">
-        <v>2801</v>
+        <v>2797</v>
       </c>
     </row>
     <row r="238" spans="1:6" ht="25.5">
@@ -25140,11 +25137,11 @@
         <v>32.299999999999997</v>
       </c>
       <c r="C238" s="10" t="s">
-        <v>2352</v>
+        <v>2351</v>
       </c>
       <c r="D238" s="10"/>
       <c r="E238" s="8" t="s">
-        <v>2801</v>
+        <v>2797</v>
       </c>
     </row>
     <row r="239" spans="1:6" ht="38.25">
@@ -25155,11 +25152,11 @@
         <v>32.4</v>
       </c>
       <c r="C239" s="10" t="s">
-        <v>2351</v>
+        <v>2350</v>
       </c>
       <c r="D239" s="10"/>
       <c r="E239" s="8" t="s">
-        <v>2801</v>
+        <v>2797</v>
       </c>
     </row>
     <row r="240" spans="1:6">
@@ -25167,7 +25164,7 @@
         <v>33</v>
       </c>
       <c r="B240" t="s">
-        <v>2350</v>
+        <v>2349</v>
       </c>
       <c r="C240" s="10"/>
       <c r="D240" s="10"/>
@@ -25180,14 +25177,14 @@
         <v>33.1</v>
       </c>
       <c r="C241" s="10" t="s">
-        <v>2349</v>
+        <v>2348</v>
       </c>
       <c r="D241" s="10"/>
       <c r="E241" s="8" t="s">
-        <v>2764</v>
+        <v>2763</v>
       </c>
       <c r="F241" s="8" t="s">
-        <v>2348</v>
+        <v>2347</v>
       </c>
     </row>
     <row r="242" spans="1:6">
@@ -25198,7 +25195,7 @@
         <v>33.200000000000003</v>
       </c>
       <c r="C242" s="10" t="s">
-        <v>2347</v>
+        <v>2346</v>
       </c>
       <c r="D242" s="10"/>
     </row>
@@ -25207,137 +25204,137 @@
         <v>34</v>
       </c>
       <c r="B243" t="s">
-        <v>2346</v>
+        <v>2345</v>
       </c>
       <c r="C243" s="10"/>
       <c r="D243" s="10"/>
     </row>
     <row r="244" spans="1:6" ht="45.95" customHeight="1">
       <c r="A244" t="s">
-        <v>2345</v>
+        <v>2344</v>
       </c>
       <c r="B244" t="s">
-        <v>2345</v>
+        <v>2344</v>
       </c>
       <c r="C244" s="10" t="s">
-        <v>2344</v>
+        <v>2343</v>
       </c>
       <c r="D244" s="10"/>
       <c r="E244" s="8" t="s">
-        <v>2802</v>
+        <v>2798</v>
       </c>
       <c r="F244" s="8" t="s">
-        <v>2343</v>
+        <v>2342</v>
       </c>
     </row>
     <row r="245" spans="1:6" ht="27" customHeight="1">
       <c r="A245" t="s">
-        <v>2342</v>
+        <v>2341</v>
       </c>
       <c r="B245" t="s">
-        <v>2342</v>
+        <v>2341</v>
       </c>
       <c r="C245" s="10" t="s">
-        <v>2341</v>
+        <v>2340</v>
       </c>
       <c r="D245" s="10"/>
       <c r="E245" s="8" t="s">
-        <v>2765</v>
+        <v>2764</v>
       </c>
     </row>
     <row r="246" spans="1:6" ht="28.5" customHeight="1">
       <c r="A246" t="s">
-        <v>2340</v>
+        <v>2339</v>
       </c>
       <c r="B246" t="s">
-        <v>2340</v>
+        <v>2339</v>
       </c>
       <c r="C246" s="10" t="s">
-        <v>2339</v>
+        <v>2338</v>
       </c>
       <c r="D246" s="10"/>
     </row>
     <row r="247" spans="1:6" ht="63.75">
       <c r="A247" t="s">
-        <v>2338</v>
+        <v>2337</v>
       </c>
       <c r="B247" t="s">
-        <v>2338</v>
+        <v>2337</v>
       </c>
       <c r="C247" s="10" t="s">
-        <v>2337</v>
+        <v>2336</v>
       </c>
       <c r="D247" s="10"/>
     </row>
     <row r="248" spans="1:6" ht="25.5">
       <c r="A248" t="s">
-        <v>2336</v>
+        <v>2335</v>
       </c>
       <c r="B248" t="s">
-        <v>2336</v>
+        <v>2335</v>
       </c>
       <c r="C248" s="10" t="s">
-        <v>2335</v>
+        <v>2334</v>
       </c>
       <c r="D248" s="10"/>
       <c r="E248" s="8" t="s">
-        <v>2764</v>
+        <v>2763</v>
       </c>
     </row>
     <row r="249" spans="1:6">
       <c r="A249" t="s">
-        <v>2334</v>
+        <v>2333</v>
       </c>
       <c r="B249" t="s">
-        <v>2334</v>
+        <v>2333</v>
       </c>
       <c r="C249" s="10" t="s">
-        <v>2333</v>
+        <v>2332</v>
       </c>
       <c r="D249" s="10"/>
       <c r="E249" s="8" t="s">
-        <v>2764</v>
+        <v>2763</v>
       </c>
     </row>
     <row r="250" spans="1:6" ht="25.5">
       <c r="A250" t="s">
-        <v>2332</v>
+        <v>2331</v>
       </c>
       <c r="B250" t="s">
-        <v>2332</v>
+        <v>2331</v>
       </c>
       <c r="C250" s="10" t="s">
-        <v>2331</v>
+        <v>2330</v>
       </c>
       <c r="D250" s="10"/>
       <c r="E250" s="8" t="s">
-        <v>2764</v>
+        <v>2763</v>
       </c>
     </row>
     <row r="251" spans="1:6" ht="51">
       <c r="A251" t="s">
-        <v>2330</v>
+        <v>2329</v>
       </c>
       <c r="B251" t="s">
-        <v>2330</v>
+        <v>2329</v>
       </c>
       <c r="C251" s="10" t="s">
-        <v>2329</v>
+        <v>2328</v>
       </c>
       <c r="D251" s="10"/>
       <c r="E251" s="8" t="s">
-        <v>2764</v>
+        <v>2763</v>
       </c>
     </row>
     <row r="252" spans="1:6" ht="38.25">
       <c r="A252" t="s">
-        <v>2328</v>
+        <v>2327</v>
       </c>
       <c r="B252" t="s">
-        <v>2328</v>
+        <v>2327</v>
       </c>
       <c r="C252" s="10" t="s">
-        <v>2327</v>
+        <v>2326</v>
       </c>
       <c r="D252" s="10"/>
       <c r="E252" s="8" t="s">
@@ -25352,7 +25349,7 @@
         <v>34.299999999999997</v>
       </c>
       <c r="C253" s="10" t="s">
-        <v>2326</v>
+        <v>2325</v>
       </c>
       <c r="D253" s="10"/>
       <c r="E253" s="8" t="s">
@@ -25364,40 +25361,40 @@
         <v>35</v>
       </c>
       <c r="B254" t="s">
-        <v>2325</v>
+        <v>2324</v>
       </c>
       <c r="C254" s="10" t="s">
-        <v>2324</v>
+        <v>2323</v>
       </c>
       <c r="D254" s="10"/>
     </row>
     <row r="255" spans="1:6" ht="45">
       <c r="A255" t="s">
-        <v>2323</v>
+        <v>2322</v>
       </c>
       <c r="B255" t="s">
-        <v>2323</v>
+        <v>2322</v>
       </c>
       <c r="C255" s="10" t="s">
-        <v>2322</v>
+        <v>2321</v>
       </c>
       <c r="D255" s="10"/>
       <c r="E255" s="8" t="s">
-        <v>2290</v>
+        <v>2289</v>
       </c>
       <c r="F255" s="8" t="s">
-        <v>2321</v>
+        <v>2320</v>
       </c>
     </row>
     <row r="256" spans="1:6" ht="30.95" customHeight="1">
       <c r="A256" t="s">
-        <v>2320</v>
+        <v>2319</v>
       </c>
       <c r="B256" t="s">
-        <v>2320</v>
+        <v>2319</v>
       </c>
       <c r="C256" s="10" t="s">
-        <v>2319</v>
+        <v>2318</v>
       </c>
       <c r="D256" s="10"/>
     </row>
@@ -25406,84 +25403,84 @@
         <v>36</v>
       </c>
       <c r="B257" s="9" t="s">
-        <v>2318</v>
+        <v>2317</v>
       </c>
       <c r="C257" s="10"/>
       <c r="D257" s="10"/>
     </row>
     <row r="258" spans="1:6" ht="63.75">
       <c r="A258" t="s">
-        <v>2317</v>
+        <v>2316</v>
       </c>
       <c r="B258" t="s">
-        <v>2317</v>
+        <v>2316</v>
       </c>
       <c r="C258" s="10" t="s">
-        <v>2316</v>
+        <v>2315</v>
       </c>
       <c r="D258" s="10"/>
       <c r="E258" s="8" t="s">
-        <v>2797</v>
+        <v>2793</v>
       </c>
     </row>
     <row r="259" spans="1:6" ht="25.5">
       <c r="A259" t="s">
-        <v>2315</v>
+        <v>2314</v>
       </c>
       <c r="B259" t="s">
-        <v>2315</v>
+        <v>2314</v>
       </c>
       <c r="C259" s="10" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
       <c r="D259" s="10"/>
       <c r="E259" s="8" t="s">
-        <v>2797</v>
+        <v>2793</v>
       </c>
     </row>
     <row r="260" spans="1:6">
       <c r="A260" t="s">
-        <v>2313</v>
+        <v>2312</v>
       </c>
       <c r="B260" t="s">
-        <v>2313</v>
+        <v>2312</v>
       </c>
       <c r="C260" s="10" t="s">
-        <v>2312</v>
+        <v>2311</v>
       </c>
       <c r="D260" s="10"/>
       <c r="E260" s="8" t="s">
-        <v>2797</v>
+        <v>2793</v>
       </c>
     </row>
     <row r="261" spans="1:6" ht="25.5">
       <c r="A261" t="s">
-        <v>2311</v>
+        <v>2310</v>
       </c>
       <c r="B261" t="s">
-        <v>2311</v>
+        <v>2310</v>
       </c>
       <c r="C261" s="10" t="s">
-        <v>2310</v>
+        <v>2309</v>
       </c>
       <c r="D261" s="10"/>
       <c r="E261" s="8" t="s">
-        <v>2797</v>
+        <v>2793</v>
       </c>
     </row>
     <row r="262" spans="1:6" ht="25.5">
       <c r="A262" t="s">
-        <v>2309</v>
+        <v>2308</v>
       </c>
       <c r="B262" t="s">
-        <v>2309</v>
+        <v>2308</v>
       </c>
       <c r="C262" s="10" t="s">
-        <v>2308</v>
+        <v>2307</v>
       </c>
       <c r="D262" s="10"/>
       <c r="E262" s="8" t="s">
-        <v>2797</v>
+        <v>2793</v>
       </c>
     </row>
     <row r="263" spans="1:6" ht="150">
@@ -25491,10 +25488,10 @@
         <v>37</v>
       </c>
       <c r="B263" s="9" t="s">
-        <v>2307</v>
+        <v>2306</v>
       </c>
       <c r="C263" s="10" t="s">
-        <v>2306</v>
+        <v>2305</v>
       </c>
       <c r="D263" s="10"/>
       <c r="E263" s="8" t="s">
@@ -25506,43 +25503,43 @@
         <v>38</v>
       </c>
       <c r="B264" s="9" t="s">
-        <v>2305</v>
+        <v>2304</v>
       </c>
       <c r="C264" s="10" t="s">
-        <v>2304</v>
+        <v>2303</v>
       </c>
       <c r="D264" s="10"/>
       <c r="E264" s="8" t="s">
-        <v>2290</v>
+        <v>2289</v>
       </c>
     </row>
     <row r="265" spans="1:6" ht="30">
       <c r="A265" t="s">
-        <v>2303</v>
+        <v>2302</v>
       </c>
       <c r="B265" t="s">
-        <v>2303</v>
+        <v>2302</v>
       </c>
       <c r="C265" s="10" t="s">
-        <v>2302</v>
+        <v>2301</v>
       </c>
       <c r="D265" s="10"/>
       <c r="E265" s="8" t="s">
-        <v>2766</v>
+        <v>2765</v>
       </c>
       <c r="F265" s="8" t="s">
-        <v>2301</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="266" spans="1:6">
       <c r="A266" t="s">
-        <v>2300</v>
+        <v>2299</v>
       </c>
       <c r="B266" t="s">
-        <v>2300</v>
+        <v>2299</v>
       </c>
       <c r="C266" s="10" t="s">
-        <v>2299</v>
+        <v>2298</v>
       </c>
       <c r="D266" s="10"/>
       <c r="E266" s="8" t="s">
@@ -25551,13 +25548,13 @@
     </row>
     <row r="267" spans="1:6" ht="25.5">
       <c r="A267" t="s">
-        <v>2298</v>
+        <v>2297</v>
       </c>
       <c r="B267" t="s">
-        <v>2298</v>
+        <v>2297</v>
       </c>
       <c r="C267" s="10" t="s">
-        <v>2297</v>
+        <v>2296</v>
       </c>
       <c r="D267" s="10"/>
       <c r="E267" s="8" t="s">
@@ -25566,32 +25563,32 @@
     </row>
     <row r="268" spans="1:6">
       <c r="A268" t="s">
-        <v>2296</v>
+        <v>2295</v>
       </c>
       <c r="B268" t="s">
-        <v>2296</v>
+        <v>2295</v>
       </c>
       <c r="C268" s="10" t="s">
-        <v>2295</v>
+        <v>2294</v>
       </c>
       <c r="D268" s="10"/>
       <c r="E268" s="8" t="s">
-        <v>2767</v>
+        <v>2766</v>
       </c>
     </row>
     <row r="269" spans="1:6">
       <c r="A269" t="s">
-        <v>2294</v>
+        <v>2293</v>
       </c>
       <c r="B269" t="s">
-        <v>2294</v>
+        <v>2293</v>
       </c>
       <c r="C269" s="10" t="s">
-        <v>2293</v>
+        <v>2292</v>
       </c>
       <c r="D269" s="10"/>
       <c r="E269" s="8" t="s">
-        <v>2768</v>
+        <v>2767</v>
       </c>
     </row>
     <row r="270" spans="1:6">
@@ -25599,7 +25596,7 @@
         <v>39</v>
       </c>
       <c r="B270" t="s">
-        <v>2292</v>
+        <v>2291</v>
       </c>
       <c r="C270" s="10"/>
       <c r="D270" s="10"/>
@@ -25612,11 +25609,11 @@
         <v>39.1</v>
       </c>
       <c r="C271" s="10" t="s">
-        <v>2291</v>
+        <v>2290</v>
       </c>
       <c r="D271" s="10"/>
       <c r="E271" s="8" t="s">
-        <v>2290</v>
+        <v>2289</v>
       </c>
     </row>
     <row r="272" spans="1:6" ht="25.5">
@@ -25627,43 +25624,43 @@
         <v>39.200000000000003</v>
       </c>
       <c r="C272" s="10" t="s">
-        <v>2289</v>
+        <v>2288</v>
       </c>
       <c r="D272" s="10"/>
     </row>
     <row r="273" spans="1:5">
       <c r="A273" t="s">
-        <v>2288</v>
+        <v>2287</v>
       </c>
       <c r="B273" t="s">
-        <v>2288</v>
+        <v>2287</v>
       </c>
       <c r="C273" s="10" t="s">
-        <v>2287</v>
+        <v>2286</v>
       </c>
       <c r="D273" s="10"/>
     </row>
     <row r="274" spans="1:5">
       <c r="A274" t="s">
-        <v>2286</v>
+        <v>2285</v>
       </c>
       <c r="B274" t="s">
-        <v>2286</v>
+        <v>2285</v>
       </c>
       <c r="C274" s="10" t="s">
-        <v>2285</v>
+        <v>2284</v>
       </c>
       <c r="D274" s="10"/>
     </row>
     <row r="275" spans="1:5">
       <c r="A275" t="s">
-        <v>2284</v>
+        <v>2283</v>
       </c>
       <c r="B275" t="s">
-        <v>2284</v>
+        <v>2283</v>
       </c>
       <c r="C275" s="10" t="s">
-        <v>2283</v>
+        <v>2282</v>
       </c>
       <c r="D275" s="10"/>
     </row>
@@ -25672,14 +25669,14 @@
         <v>40</v>
       </c>
       <c r="B276" t="s">
-        <v>2282</v>
+        <v>2281</v>
       </c>
       <c r="C276" s="10" t="s">
-        <v>2281</v>
+        <v>2280</v>
       </c>
       <c r="D276" s="10"/>
       <c r="E276" s="8" t="s">
-        <v>2767</v>
+        <v>2766</v>
       </c>
     </row>
     <row r="277" spans="1:5" ht="89.25">
@@ -25687,10 +25684,10 @@
         <v>41</v>
       </c>
       <c r="B277" s="14" t="s">
-        <v>2280</v>
+        <v>2279</v>
       </c>
       <c r="C277" s="10" t="s">
-        <v>2279</v>
+        <v>2278</v>
       </c>
       <c r="D277" s="10"/>
     </row>
@@ -25699,10 +25696,10 @@
         <v>42</v>
       </c>
       <c r="B278" s="14" t="s">
-        <v>2278</v>
+        <v>2277</v>
       </c>
       <c r="C278" s="10" t="s">
-        <v>2277</v>
+        <v>2276</v>
       </c>
       <c r="D278" s="10"/>
     </row>
@@ -25711,10 +25708,10 @@
         <v>43</v>
       </c>
       <c r="B279" s="14" t="s">
-        <v>2276</v>
+        <v>2275</v>
       </c>
       <c r="C279" s="10" t="s">
-        <v>2275</v>
+        <v>2274</v>
       </c>
       <c r="D279" s="10"/>
     </row>
@@ -25723,10 +25720,10 @@
         <v>44</v>
       </c>
       <c r="B280" s="14" t="s">
-        <v>2274</v>
+        <v>2273</v>
       </c>
       <c r="C280" s="10" t="s">
-        <v>2273</v>
+        <v>2272</v>
       </c>
       <c r="D280" s="10"/>
     </row>
@@ -25735,10 +25732,10 @@
         <v>45</v>
       </c>
       <c r="B281" s="14" t="s">
-        <v>2272</v>
+        <v>2271</v>
       </c>
       <c r="C281" s="10" t="s">
-        <v>2271</v>
+        <v>2270</v>
       </c>
       <c r="D281" s="10"/>
     </row>
@@ -25747,10 +25744,10 @@
         <v>46</v>
       </c>
       <c r="B282" s="14" t="s">
-        <v>2270</v>
+        <v>2269</v>
       </c>
       <c r="C282" s="10" t="s">
-        <v>2269</v>
+        <v>2268</v>
       </c>
       <c r="D282" s="10"/>
     </row>
@@ -25759,10 +25756,10 @@
         <v>47</v>
       </c>
       <c r="B283" s="14" t="s">
-        <v>2268</v>
+        <v>2267</v>
       </c>
       <c r="C283" s="10" t="s">
-        <v>2267</v>
+        <v>2266</v>
       </c>
       <c r="D283" s="10"/>
     </row>
@@ -25771,10 +25768,10 @@
         <v>48</v>
       </c>
       <c r="B284" s="14" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
       <c r="C284" s="10" t="s">
-        <v>2265</v>
+        <v>2264</v>
       </c>
       <c r="D284" s="10"/>
     </row>
@@ -25783,10 +25780,10 @@
         <v>49</v>
       </c>
       <c r="B285" s="14" t="s">
-        <v>2264</v>
+        <v>2263</v>
       </c>
       <c r="C285" s="10" t="s">
-        <v>2263</v>
+        <v>2262</v>
       </c>
       <c r="D285" s="10"/>
     </row>
@@ -25795,10 +25792,10 @@
         <v>50</v>
       </c>
       <c r="B286" s="9" t="s">
-        <v>2262</v>
+        <v>2261</v>
       </c>
       <c r="C286" s="10" t="s">
-        <v>2261</v>
+        <v>2260</v>
       </c>
       <c r="D286" s="10"/>
       <c r="E286" s="8" t="s">
@@ -25810,10 +25807,10 @@
         <v>51</v>
       </c>
       <c r="B287" s="14" t="s">
-        <v>2260</v>
+        <v>2259</v>
       </c>
       <c r="C287" s="10" t="s">
-        <v>2259</v>
+        <v>2258</v>
       </c>
       <c r="D287" s="10"/>
     </row>
@@ -25822,10 +25819,10 @@
         <v>52</v>
       </c>
       <c r="B288" s="14" t="s">
-        <v>2258</v>
+        <v>2257</v>
       </c>
       <c r="C288" s="10" t="s">
-        <v>2257</v>
+        <v>2256</v>
       </c>
       <c r="D288" s="10"/>
     </row>
@@ -25834,10 +25831,10 @@
         <v>53</v>
       </c>
       <c r="B289" s="14" t="s">
-        <v>2256</v>
+        <v>2255</v>
       </c>
       <c r="C289" s="10" t="s">
-        <v>2255</v>
+        <v>2254</v>
       </c>
       <c r="D289" s="10"/>
     </row>
@@ -25846,10 +25843,10 @@
         <v>54</v>
       </c>
       <c r="B290" s="14" t="s">
-        <v>2254</v>
+        <v>2253</v>
       </c>
       <c r="C290" s="10" t="s">
-        <v>2253</v>
+        <v>2252</v>
       </c>
       <c r="D290" s="10"/>
     </row>
@@ -25858,10 +25855,10 @@
         <v>55</v>
       </c>
       <c r="B291" s="14" t="s">
-        <v>2252</v>
+        <v>2251</v>
       </c>
       <c r="C291" s="10" t="s">
-        <v>2251</v>
+        <v>2250</v>
       </c>
       <c r="D291" s="10"/>
     </row>
@@ -25870,10 +25867,10 @@
         <v>56</v>
       </c>
       <c r="B292" s="14" t="s">
-        <v>2250</v>
+        <v>2249</v>
       </c>
       <c r="C292" s="10" t="s">
-        <v>2249</v>
+        <v>2248</v>
       </c>
       <c r="D292" s="10"/>
     </row>
@@ -25882,7 +25879,7 @@
         <v>57</v>
       </c>
       <c r="B293" s="10" t="s">
-        <v>2248</v>
+        <v>2247</v>
       </c>
       <c r="C293" s="10"/>
       <c r="D293" s="10"/>
@@ -25895,22 +25892,22 @@
         <v>57.1</v>
       </c>
       <c r="C294" s="10" t="s">
-        <v>2247</v>
+        <v>2246</v>
       </c>
       <c r="D294" s="10"/>
       <c r="E294" s="8" t="s">
-        <v>2769</v>
+        <v>2768</v>
       </c>
     </row>
     <row r="295" spans="1:5" ht="27.95" customHeight="1">
       <c r="A295" t="s">
-        <v>2246</v>
+        <v>2245</v>
       </c>
       <c r="B295" t="s">
-        <v>2246</v>
+        <v>2245</v>
       </c>
       <c r="C295" s="10" t="s">
-        <v>2245</v>
+        <v>2244</v>
       </c>
       <c r="D295" s="10"/>
       <c r="E295" s="8" t="s">
@@ -25919,28 +25916,28 @@
     </row>
     <row r="296" spans="1:5">
       <c r="A296" t="s">
-        <v>2244</v>
+        <v>2243</v>
       </c>
       <c r="B296" t="s">
-        <v>2244</v>
+        <v>2243</v>
       </c>
       <c r="C296" s="10" t="s">
-        <v>2243</v>
+        <v>2242</v>
       </c>
       <c r="D296" s="10"/>
       <c r="E296" s="8" t="s">
-        <v>2760</v>
+        <v>2759</v>
       </c>
     </row>
     <row r="297" spans="1:5">
       <c r="A297" t="s">
-        <v>2242</v>
+        <v>2241</v>
       </c>
       <c r="B297" t="s">
-        <v>2242</v>
+        <v>2241</v>
       </c>
       <c r="C297" s="10" t="s">
-        <v>2241</v>
+        <v>2240</v>
       </c>
       <c r="D297" s="10"/>
       <c r="E297" s="8" t="s">
@@ -25949,28 +25946,28 @@
     </row>
     <row r="298" spans="1:5">
       <c r="A298" t="s">
-        <v>2240</v>
+        <v>2239</v>
       </c>
       <c r="B298" t="s">
-        <v>2240</v>
+        <v>2239</v>
       </c>
       <c r="C298" s="10" t="s">
-        <v>2239</v>
+        <v>2238</v>
       </c>
       <c r="D298" s="10"/>
       <c r="E298" s="8" t="s">
-        <v>2803</v>
+        <v>2799</v>
       </c>
     </row>
     <row r="299" spans="1:5">
       <c r="A299" t="s">
-        <v>2238</v>
+        <v>2237</v>
       </c>
       <c r="B299" t="s">
-        <v>2238</v>
+        <v>2237</v>
       </c>
       <c r="C299" s="10" t="s">
-        <v>2237</v>
+        <v>2236</v>
       </c>
       <c r="D299" s="10"/>
       <c r="E299" s="8" t="s">
@@ -25985,68 +25982,68 @@
         <v>57.2</v>
       </c>
       <c r="C300" s="10" t="s">
-        <v>2236</v>
+        <v>2235</v>
       </c>
       <c r="D300" s="10"/>
     </row>
     <row r="301" spans="1:5" ht="30">
       <c r="A301" t="s">
-        <v>2235</v>
+        <v>2234</v>
       </c>
       <c r="B301" t="s">
-        <v>2235</v>
+        <v>2234</v>
       </c>
       <c r="C301" s="10" t="s">
-        <v>2234</v>
+        <v>2233</v>
       </c>
       <c r="D301" s="10"/>
       <c r="E301" s="8" t="s">
-        <v>2804</v>
+        <v>2800</v>
       </c>
     </row>
     <row r="302" spans="1:5">
       <c r="A302" t="s">
-        <v>2233</v>
+        <v>2232</v>
       </c>
       <c r="B302" t="s">
-        <v>2233</v>
+        <v>2232</v>
       </c>
       <c r="C302" s="10" t="s">
-        <v>2232</v>
+        <v>2231</v>
       </c>
       <c r="D302" s="10"/>
       <c r="E302" s="8" t="s">
-        <v>2770</v>
-      </c>
-    </row>
-    <row r="303" spans="1:5" ht="45">
+        <v>2769</v>
+      </c>
+    </row>
+    <row r="303" spans="1:5" ht="30">
       <c r="A303" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
       <c r="B303" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
       <c r="C303" s="10" t="s">
-        <v>2230</v>
+        <v>2229</v>
       </c>
       <c r="D303" s="10"/>
       <c r="E303" s="8" t="s">
-        <v>2758</v>
+        <v>2757</v>
       </c>
     </row>
     <row r="304" spans="1:5">
       <c r="A304" t="s">
-        <v>2229</v>
+        <v>2228</v>
       </c>
       <c r="B304" t="s">
-        <v>2229</v>
+        <v>2228</v>
       </c>
       <c r="C304" s="10" t="s">
-        <v>2228</v>
+        <v>2227</v>
       </c>
       <c r="D304" s="10"/>
       <c r="E304" s="8" t="s">
-        <v>2764</v>
+        <v>2763</v>
       </c>
     </row>
     <row r="305" spans="1:6">
@@ -26057,79 +26054,79 @@
         <v>57.3</v>
       </c>
       <c r="C305" s="10" t="s">
-        <v>2227</v>
+        <v>2226</v>
       </c>
       <c r="D305" s="10"/>
     </row>
     <row r="306" spans="1:6" ht="38.25">
       <c r="A306" t="s">
-        <v>2226</v>
+        <v>2225</v>
       </c>
       <c r="B306" t="s">
-        <v>2226</v>
+        <v>2225</v>
       </c>
       <c r="C306" s="10" t="s">
-        <v>2225</v>
+        <v>2224</v>
       </c>
       <c r="D306" s="10"/>
     </row>
     <row r="307" spans="1:6" ht="38.25">
       <c r="A307" t="s">
-        <v>2224</v>
+        <v>2223</v>
       </c>
       <c r="B307" t="s">
-        <v>2224</v>
+        <v>2223</v>
       </c>
       <c r="C307" s="10" t="s">
-        <v>2223</v>
+        <v>2222</v>
       </c>
       <c r="D307" s="10"/>
     </row>
     <row r="308" spans="1:6">
       <c r="A308" t="s">
-        <v>2222</v>
+        <v>2221</v>
       </c>
       <c r="B308" t="s">
-        <v>2222</v>
+        <v>2221</v>
       </c>
       <c r="C308" s="10" t="s">
-        <v>2221</v>
+        <v>2220</v>
       </c>
       <c r="D308" s="10"/>
     </row>
     <row r="309" spans="1:6" ht="25.5">
       <c r="A309" t="s">
-        <v>2220</v>
+        <v>2219</v>
       </c>
       <c r="B309" t="s">
-        <v>2220</v>
+        <v>2219</v>
       </c>
       <c r="C309" s="10" t="s">
-        <v>2219</v>
+        <v>2218</v>
       </c>
       <c r="D309" s="10"/>
     </row>
     <row r="310" spans="1:6">
       <c r="A310" t="s">
-        <v>2218</v>
+        <v>2217</v>
       </c>
       <c r="B310" t="s">
-        <v>2218</v>
+        <v>2217</v>
       </c>
       <c r="C310" s="10" t="s">
-        <v>2217</v>
+        <v>2216</v>
       </c>
       <c r="D310" s="10"/>
     </row>
     <row r="311" spans="1:6" ht="25.5">
       <c r="A311" t="s">
-        <v>2216</v>
+        <v>2215</v>
       </c>
       <c r="B311" t="s">
-        <v>2216</v>
+        <v>2215</v>
       </c>
       <c r="C311" s="10" t="s">
-        <v>2215</v>
+        <v>2214</v>
       </c>
       <c r="D311" s="10"/>
     </row>
@@ -26138,14 +26135,14 @@
         <v>58</v>
       </c>
       <c r="B312" s="9" t="s">
-        <v>2214</v>
+        <v>2213</v>
       </c>
       <c r="C312" s="10" t="s">
-        <v>2213</v>
+        <v>2212</v>
       </c>
       <c r="D312" s="10"/>
       <c r="E312" s="8" t="s">
-        <v>2771</v>
+        <v>2770</v>
       </c>
     </row>
     <row r="313" spans="1:6" ht="55.5" customHeight="1">
@@ -26153,14 +26150,14 @@
         <v>59</v>
       </c>
       <c r="B313" s="9" t="s">
-        <v>2212</v>
+        <v>2211</v>
       </c>
       <c r="C313" s="10" t="s">
-        <v>2211</v>
+        <v>2210</v>
       </c>
       <c r="D313" s="10"/>
       <c r="E313" s="8" t="s">
-        <v>2772</v>
+        <v>2771</v>
       </c>
     </row>
     <row r="314" spans="1:6" ht="180">
@@ -26168,17 +26165,17 @@
         <v>60</v>
       </c>
       <c r="B314" s="9" t="s">
-        <v>2210</v>
+        <v>2209</v>
       </c>
       <c r="C314" s="10" t="s">
-        <v>2209</v>
+        <v>2208</v>
       </c>
       <c r="D314" s="10"/>
       <c r="E314" s="8" t="s">
-        <v>2773</v>
+        <v>2772</v>
       </c>
       <c r="F314" s="8" t="s">
-        <v>2208</v>
+        <v>2207</v>
       </c>
     </row>
     <row r="315" spans="1:6" ht="52.5" customHeight="1">
@@ -26186,14 +26183,14 @@
         <v>61</v>
       </c>
       <c r="B315" s="9" t="s">
-        <v>2207</v>
+        <v>2206</v>
       </c>
       <c r="C315" s="10" t="s">
-        <v>2206</v>
+        <v>2205</v>
       </c>
       <c r="D315" s="10"/>
       <c r="E315" s="8" t="s">
-        <v>2773</v>
+        <v>2772</v>
       </c>
     </row>
     <row r="316" spans="1:6" ht="140.25">
@@ -26201,14 +26198,14 @@
         <v>62</v>
       </c>
       <c r="B316" s="9" t="s">
-        <v>2205</v>
+        <v>2204</v>
       </c>
       <c r="C316" s="10" t="s">
-        <v>2204</v>
+        <v>2203</v>
       </c>
       <c r="D316" s="10"/>
       <c r="E316" s="8" t="s">
-        <v>2203</v>
+        <v>10</v>
       </c>
     </row>
     <row r="317" spans="1:6" ht="324" customHeight="1">
@@ -26245,7 +26242,7 @@
       </c>
       <c r="D319" s="10"/>
       <c r="E319" s="8" t="s">
-        <v>2774</v>
+        <v>2773</v>
       </c>
     </row>
     <row r="320" spans="1:6" ht="15.6" customHeight="1">
@@ -26290,7 +26287,7 @@
       </c>
       <c r="D322" s="10"/>
       <c r="E322" s="8" t="s">
-        <v>2775</v>
+        <v>2774</v>
       </c>
     </row>
     <row r="323" spans="1:5" ht="15.6" customHeight="1">
@@ -26305,7 +26302,7 @@
       </c>
       <c r="D323" s="10"/>
       <c r="E323" s="8" t="s">
-        <v>2775</v>
+        <v>2774</v>
       </c>
     </row>
     <row r="324" spans="1:5" ht="15.6" customHeight="1">
@@ -26320,7 +26317,7 @@
       </c>
       <c r="D324" s="10"/>
       <c r="E324" s="8" t="s">
-        <v>2775</v>
+        <v>2774</v>
       </c>
     </row>
     <row r="325" spans="1:5" ht="29.1" customHeight="1">
@@ -26335,7 +26332,7 @@
       </c>
       <c r="D325" s="10"/>
       <c r="E325" s="8" t="s">
-        <v>2776</v>
+        <v>2775</v>
       </c>
     </row>
     <row r="326" spans="1:5" ht="15.6" customHeight="1">
@@ -26350,7 +26347,7 @@
       </c>
       <c r="D326" s="10"/>
       <c r="E326" s="8" t="s">
-        <v>2805</v>
+        <v>2801</v>
       </c>
     </row>
     <row r="327" spans="1:5" ht="15.6" customHeight="1">
@@ -26365,7 +26362,7 @@
       </c>
       <c r="D327" s="10"/>
       <c r="E327" s="8" t="s">
-        <v>2775</v>
+        <v>2774</v>
       </c>
     </row>
     <row r="328" spans="1:5" ht="15.6" customHeight="1">
@@ -26380,7 +26377,7 @@
       </c>
       <c r="D328" s="10"/>
       <c r="E328" s="8" t="s">
-        <v>2776</v>
+        <v>2775</v>
       </c>
     </row>
     <row r="329" spans="1:5" ht="26.1" customHeight="1">
@@ -26395,7 +26392,7 @@
       </c>
       <c r="D329" s="10"/>
       <c r="E329" s="8" t="s">
-        <v>2775</v>
+        <v>2774</v>
       </c>
     </row>
     <row r="330" spans="1:5" ht="47.45" customHeight="1">
@@ -26410,7 +26407,7 @@
       </c>
       <c r="D330" s="10"/>
       <c r="E330" s="8" t="s">
-        <v>2800</v>
+        <v>2796</v>
       </c>
     </row>
     <row r="331" spans="1:5" ht="43.5" customHeight="1">
@@ -26425,7 +26422,7 @@
       </c>
       <c r="D331" s="10"/>
       <c r="E331" s="8" t="s">
-        <v>2800</v>
+        <v>2796</v>
       </c>
     </row>
     <row r="332" spans="1:5" ht="15.6" customHeight="1">
@@ -26467,7 +26464,7 @@
       </c>
       <c r="D334" s="10"/>
       <c r="E334" s="8" t="s">
-        <v>2777</v>
+        <v>2806</v>
       </c>
     </row>
     <row r="335" spans="1:5" ht="60">
@@ -26608,7 +26605,7 @@
       </c>
       <c r="D345" s="10"/>
       <c r="E345" s="8" t="s">
-        <v>2806</v>
+        <v>2802</v>
       </c>
     </row>
     <row r="346" spans="1:6" ht="75">
@@ -26683,7 +26680,7 @@
       </c>
       <c r="D351" s="10"/>
       <c r="E351" s="8" t="s">
-        <v>2778</v>
+        <v>2776</v>
       </c>
     </row>
     <row r="352" spans="1:6" ht="42.95" customHeight="1">
@@ -26698,7 +26695,7 @@
       </c>
       <c r="D352" s="10"/>
       <c r="E352" s="8" t="s">
-        <v>2779</v>
+        <v>2777</v>
       </c>
       <c r="F352" s="8" t="s">
         <v>2138</v>
@@ -26716,7 +26713,7 @@
       </c>
       <c r="D353" s="10"/>
       <c r="E353" s="8" t="s">
-        <v>2807</v>
+        <v>2803</v>
       </c>
     </row>
     <row r="354" spans="1:6" ht="165.75">
@@ -26731,7 +26728,7 @@
       </c>
       <c r="D354" s="10"/>
       <c r="E354" s="8" t="s">
-        <v>2807</v>
+        <v>2803</v>
       </c>
     </row>
     <row r="355" spans="1:6" ht="120">
@@ -26746,7 +26743,7 @@
       </c>
       <c r="D355" s="10"/>
       <c r="E355" s="8" t="s">
-        <v>2788</v>
+        <v>2785</v>
       </c>
     </row>
     <row r="356" spans="1:6" ht="75">
@@ -26806,7 +26803,7 @@
       </c>
       <c r="D360" s="10"/>
       <c r="E360" s="8" t="s">
-        <v>2788</v>
+        <v>2785</v>
       </c>
       <c r="F360" s="8" t="s">
         <v>2122</v>
@@ -26824,7 +26821,7 @@
       </c>
       <c r="D361" s="10"/>
       <c r="E361" s="8" t="s">
-        <v>2788</v>
+        <v>2785</v>
       </c>
     </row>
     <row r="362" spans="1:6" ht="409.5">
@@ -26839,7 +26836,7 @@
       </c>
       <c r="D362" s="10"/>
       <c r="E362" s="8" t="s">
-        <v>2788</v>
+        <v>2785</v>
       </c>
     </row>
     <row r="363" spans="1:6" ht="408.75" customHeight="1">
@@ -26854,7 +26851,7 @@
       </c>
       <c r="D363" s="10"/>
       <c r="E363" s="8" t="s">
-        <v>2788</v>
+        <v>2785</v>
       </c>
     </row>
     <row r="364" spans="1:6" ht="120">
@@ -30354,6 +30351,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_STS_x0020_Hashtags xmlns="b38e6452-0983-483a-b0d4-324af6d44e4d"/>
+    <MediaServiceKeyPoints xmlns="b38e6452-0983-483a-b0d4-324af6d44e4d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010072B72D3E1CFCDD40BC0C6D9CCD45E0BB" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1091b63e79dc81a90741573e3164413c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="759c4387-f01d-437d-8a5d-56d9b05a6914" xmlns:ns4="b38e6452-0983-483a-b0d4-324af6d44e4d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7010e408eae2039b0bc4bac303a742c1" ns3:_="" ns4:_="">
     <xsd:import namespace="759c4387-f01d-437d-8a5d-56d9b05a6914"/>
@@ -30604,15 +30610,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_STS_x0020_Hashtags xmlns="b38e6452-0983-483a-b0d4-324af6d44e4d"/>
-    <MediaServiceKeyPoints xmlns="b38e6452-0983-483a-b0d4-324af6d44e4d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A59176D2-D324-41A5-A125-AC358C249804}">
   <ds:schemaRefs>
@@ -30622,6 +30619,16 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71725466-609F-438E-9D55-68B1CE9C392F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b38e6452-0983-483a-b0d4-324af6d44e4d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC11F96C-E600-42F3-BB18-A579B8C44705}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -30638,14 +30645,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71725466-609F-438E-9D55-68B1CE9C392F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b38e6452-0983-483a-b0d4-324af6d44e4d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fixed formatting error in PDPB 64.4b to remove extra "."
</commit_message>
<xml_diff>
--- a/src/assets/database.xlsx
+++ b/src/assets/database.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B870772E-9DFB-4C9C-82DC-65823EEFD081}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AB0553-5668-4244-B2CE-3FB7FE36B669}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5130" uniqueCount="2807">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5130" uniqueCount="2808">
   <si>
     <t>id</t>
   </si>
@@ -9696,6 +9696,9 @@
   </si>
   <si>
     <t>5.2.1;5.2.2</t>
+  </si>
+  <si>
+    <t>7.3.2;7.3.3;7.2.8;8.3.1;6.15.2</t>
   </si>
 </sst>
 </file>
@@ -21721,8 +21724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24BA70E6-9548-4D87-8A65-060EC90D2814}">
   <dimension ref="A1:F664"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A347" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E335" sqref="E335"/>
+    <sheetView tabSelected="1" topLeftCell="A318" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E328" sqref="E328"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -26377,7 +26380,7 @@
       </c>
       <c r="D328" s="10"/>
       <c r="E328" s="8" t="s">
-        <v>2775</v>
+        <v>2807</v>
       </c>
     </row>
     <row r="329" spans="1:5" ht="26.1" customHeight="1">
@@ -30351,15 +30354,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_STS_x0020_Hashtags xmlns="b38e6452-0983-483a-b0d4-324af6d44e4d"/>
-    <MediaServiceKeyPoints xmlns="b38e6452-0983-483a-b0d4-324af6d44e4d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010072B72D3E1CFCDD40BC0C6D9CCD45E0BB" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1091b63e79dc81a90741573e3164413c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="759c4387-f01d-437d-8a5d-56d9b05a6914" xmlns:ns4="b38e6452-0983-483a-b0d4-324af6d44e4d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7010e408eae2039b0bc4bac303a742c1" ns3:_="" ns4:_="">
     <xsd:import namespace="759c4387-f01d-437d-8a5d-56d9b05a6914"/>
@@ -30610,6 +30604,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_STS_x0020_Hashtags xmlns="b38e6452-0983-483a-b0d4-324af6d44e4d"/>
+    <MediaServiceKeyPoints xmlns="b38e6452-0983-483a-b0d4-324af6d44e4d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A59176D2-D324-41A5-A125-AC358C249804}">
   <ds:schemaRefs>
@@ -30619,16 +30622,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71725466-609F-438E-9D55-68B1CE9C392F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b38e6452-0983-483a-b0d4-324af6d44e4d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC11F96C-E600-42F3-BB18-A579B8C44705}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -30645,4 +30638,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71725466-609F-438E-9D55-68B1CE9C392F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b38e6452-0983-483a-b0d4-324af6d44e4d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added NIST PF unedited
</commit_message>
<xml_diff>
--- a/src/assets/database.xlsx
+++ b/src/assets/database.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AB0553-5668-4244-B2CE-3FB7FE36B669}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD34D380-A084-48C4-9D44-C54A99B3DBB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ChangeLog" sheetId="11" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="California CCPA " sheetId="8" r:id="rId10"/>
     <sheet name="Brazil " sheetId="9" r:id="rId11"/>
     <sheet name="GDPR" sheetId="10" r:id="rId12"/>
+    <sheet name="NIST Privacy Framework" sheetId="13" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="_Toc506801608" localSheetId="3">'Australia '!$C$2</definedName>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5130" uniqueCount="2808">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5599" uniqueCount="3213">
   <si>
     <t>id</t>
   </si>
@@ -9699,6 +9700,1221 @@
   </si>
   <si>
     <t>7.3.2;7.3.3;7.2.8;8.3.1;6.15.2</t>
+  </si>
+  <si>
+    <t>ID_P</t>
+  </si>
+  <si>
+    <t>ID-P</t>
+  </si>
+  <si>
+    <t>IDENTIFY-P: Develop the organizational understanding to manage privacy risk for individuals arising from data processing.</t>
+  </si>
+  <si>
+    <t>ID_P.IM_P</t>
+  </si>
+  <si>
+    <t>ID.IM-P</t>
+  </si>
+  <si>
+    <t>Inventory and Mapping: Data processing by systems, products, or services is understood and informs the management of privacy risk.</t>
+  </si>
+  <si>
+    <t>ID_P.IM_P.P1</t>
+  </si>
+  <si>
+    <t>ID.IM-P1</t>
+  </si>
+  <si>
+    <t>Systems/products/services that process data are inventoried.</t>
+  </si>
+  <si>
+    <t>ID_P.IM_P.P2</t>
+  </si>
+  <si>
+    <t>ID.IM-P2</t>
+  </si>
+  <si>
+    <t>Owners or operators (e.g., the organization or third parties such as service providers, partners, customers, and developers) and their roles with respect to the systems/products/services and components (e.g., internal or external) that process data are inventoried</t>
+  </si>
+  <si>
+    <t>5.2.3;7.2.8;8.2.6</t>
+  </si>
+  <si>
+    <t>ID_P.IM_P.P3</t>
+  </si>
+  <si>
+    <t>ID.IM-P3</t>
+  </si>
+  <si>
+    <t>Categories of individuals (e.g., customers, employees or prospective employees, consumers) whose data are being processed are inventoried</t>
+  </si>
+  <si>
+    <t>ID_P.IM_P.P4</t>
+  </si>
+  <si>
+    <t>ID.IM-P4</t>
+  </si>
+  <si>
+    <t>Data actions of the systems/products/services are inventoried.</t>
+  </si>
+  <si>
+    <t>ID_P.IM_P.P5</t>
+  </si>
+  <si>
+    <t>ID.IM-P5</t>
+  </si>
+  <si>
+    <t>The purposes for the data actions are inventoried.</t>
+  </si>
+  <si>
+    <t>7.2.1;8.2.2;7.2.5</t>
+  </si>
+  <si>
+    <t>ID_P.IM_P.P6</t>
+  </si>
+  <si>
+    <t>ID.IM-P6</t>
+  </si>
+  <si>
+    <t>Data elements within the data actions are inventoried.</t>
+  </si>
+  <si>
+    <t>7.2.5;7.2.8;8.2.6</t>
+  </si>
+  <si>
+    <t>ID_P.IM_P.P7</t>
+  </si>
+  <si>
+    <t>ID.IM-P7</t>
+  </si>
+  <si>
+    <t>The data processing environment is identified (e.g., geographic location, internal, cloud, third parties).</t>
+  </si>
+  <si>
+    <t>5.2.3;7.2.5;7.2.8;8.2.5;8.2.6</t>
+  </si>
+  <si>
+    <t>ID_P.IM_P.P8</t>
+  </si>
+  <si>
+    <t>ID.IM-P8</t>
+  </si>
+  <si>
+    <t>Data processing is mapped, illustrating the data actions and associated data elements for systems/products/services, including components; roles of the component owners/operators; and interactions of individuals or third parties with the systems/products/services.</t>
+  </si>
+  <si>
+    <t>ID_P.BE_P</t>
+  </si>
+  <si>
+    <t>ID.BE-P</t>
+  </si>
+  <si>
+    <t>Business Environment: The organization’s mission, objectives, stakeholders, and activities are understood and prioritized; this information is used to inform privacy roles, responsibilities, and risk management decisions.</t>
+  </si>
+  <si>
+    <t>ID_P.BE_P.P1</t>
+  </si>
+  <si>
+    <t>ID.BE-P1</t>
+  </si>
+  <si>
+    <t>The organization’s role in the data processing ecosystem is identified and communicated.</t>
+  </si>
+  <si>
+    <t>5.2.1;7.3.3;8.3.1</t>
+  </si>
+  <si>
+    <t>ID_P.BE_P.P2</t>
+  </si>
+  <si>
+    <t>ID.BE-P2</t>
+  </si>
+  <si>
+    <t>Priorities for organizational mission, objectives, and activities are established and communicated.</t>
+  </si>
+  <si>
+    <t>ID_P.BE_P.P3</t>
+  </si>
+  <si>
+    <t>ID.BE-P3</t>
+  </si>
+  <si>
+    <t>Systems/products/services that support organizational priorities are identified and key requirements communicated.</t>
+  </si>
+  <si>
+    <t>5.2.1;5.2.4</t>
+  </si>
+  <si>
+    <t>ID_P.RA_P</t>
+  </si>
+  <si>
+    <t>ID.RA-P</t>
+  </si>
+  <si>
+    <t>Risk Assessment: The organization understands the privacy risks to individuals and how such privacy risks may create follow-on impacts on organizational operations, including mission, functions, other risk management priorities (e.g. compliance, financial), reputation, workforce, and culture.</t>
+  </si>
+  <si>
+    <t>ID_P.RA_P.P1</t>
+  </si>
+  <si>
+    <t>ID.RA-P1</t>
+  </si>
+  <si>
+    <t>Contextual factors related to the systems/products/services and the data actions are identified (e.g., individuals’ demographics and privacy interests or perceptions, data sensitivity, visibility of data processing to individuals and third parties).</t>
+  </si>
+  <si>
+    <t>ID_P.RA_P.P2</t>
+  </si>
+  <si>
+    <t>ID.RA-P2</t>
+  </si>
+  <si>
+    <t>Data analytic inputs and outputs are identified and evaluated for bias.</t>
+  </si>
+  <si>
+    <t>6.11.2.1;6.11.2.5;7.3.10</t>
+  </si>
+  <si>
+    <t>ID_P.RA_P.P3</t>
+  </si>
+  <si>
+    <t>ID.RA-P3</t>
+  </si>
+  <si>
+    <t>Potential problematic data actions and associated problems are identified.</t>
+  </si>
+  <si>
+    <t>ID_P.RA_P.P4</t>
+  </si>
+  <si>
+    <t>ID.RA-P4</t>
+  </si>
+  <si>
+    <t>Problematic data actions, likelihoods, and impacts are used to determine and prioritize risk.</t>
+  </si>
+  <si>
+    <t>ID_P.RA_P.P5</t>
+  </si>
+  <si>
+    <t>ID.RA-P5</t>
+  </si>
+  <si>
+    <t>Risk responses are identified, prioritized, and implemented.</t>
+  </si>
+  <si>
+    <t>5.4.1.2;5.4.1.3</t>
+  </si>
+  <si>
+    <t>ID_P.DE_P</t>
+  </si>
+  <si>
+    <t>ID.DE-P</t>
+  </si>
+  <si>
+    <t>Data Processing Ecosystem Risk Management (ID.DE-P): The organization’s priorities, constraints, risk tolerances, and assumptions are established and used to support risk decisions associated with managing privacy risk and third parties within the data processing ecosystem. The organization has established and implemented the processes to identify, assess, and manage privacy risks within the data processing ecosystem.</t>
+  </si>
+  <si>
+    <t>ID_P.DE_P.P1</t>
+  </si>
+  <si>
+    <t>ID.DE-P1</t>
+  </si>
+  <si>
+    <t>Data processing ecosystem risk management processes are identified, established, assessed, managed, and agreed to by organizational stakeholders.</t>
+  </si>
+  <si>
+    <t>ID_P.DE_P.P2</t>
+  </si>
+  <si>
+    <t>ID.DE-P2</t>
+  </si>
+  <si>
+    <t>Data processing ecosystem parties (e.g., service providers, customers, partners, product manufacturers, application developers) are identified, prioritized, and assessed using a privacy risk assessment process.</t>
+  </si>
+  <si>
+    <t>ID_P.DE_P.P3</t>
+  </si>
+  <si>
+    <t>ID.DE-P3</t>
+  </si>
+  <si>
+    <t>Contracts with data processing ecosystem parties are used to implement appropriate measures designed to meet the objectives of an organization’s privacy program.</t>
+  </si>
+  <si>
+    <t>6.12.1.2;7.2.7;7.2.6;8.2.1</t>
+  </si>
+  <si>
+    <t>ID_P.DE_P.P4</t>
+  </si>
+  <si>
+    <t>ID.DE-P4</t>
+  </si>
+  <si>
+    <t>Interoperability frameworks or similar multi-party approaches are used to manage data processing ecosystem privacy risks.</t>
+  </si>
+  <si>
+    <t>ID_P.DE_P.P5</t>
+  </si>
+  <si>
+    <t>ID.DE-P5</t>
+  </si>
+  <si>
+    <t>Data processing ecosystem parties are routinely assessed using audits, test results, or other forms of evaluations to confirm they are meeting their contractual or framework obligations.</t>
+  </si>
+  <si>
+    <t>GV_P</t>
+  </si>
+  <si>
+    <t>GV-P</t>
+  </si>
+  <si>
+    <t>GOVERN-P: Develop and implement the organizational governance structure to enable an ongoing understanding of the organization’s risk management priorities that are informed by privacy risk.</t>
+  </si>
+  <si>
+    <t>GV_P.PP_P</t>
+  </si>
+  <si>
+    <t>GV.PP-P</t>
+  </si>
+  <si>
+    <t>Governance Policies, Processes, and Procedures: The policies, processes, and procedures to manage and monitor the organization’s regulatory, legal, risk, environmental, and operational requirements are</t>
+  </si>
+  <si>
+    <t>GV_P.PP_P.P1</t>
+  </si>
+  <si>
+    <t>GV.PP-P1</t>
+  </si>
+  <si>
+    <t>Organizational privacy values and policies (e.g., conditions on data processing, individuals’ prerogatives with respect to data processing) are established and communicated.</t>
+  </si>
+  <si>
+    <t>GV_P.PP_P.P2</t>
+  </si>
+  <si>
+    <t>GV.PP-P2</t>
+  </si>
+  <si>
+    <t>Processes to instill organizational privacy values within system/product/service development and operations are established and in place.</t>
+  </si>
+  <si>
+    <t>GV_P.PP_P.P3</t>
+  </si>
+  <si>
+    <t>GV.PP-P3</t>
+  </si>
+  <si>
+    <t>Roles and responsibilities for the workforce are established with respect to privacy.</t>
+  </si>
+  <si>
+    <t>GV_P.PP_P.P4</t>
+  </si>
+  <si>
+    <t>GV.PP-P4</t>
+  </si>
+  <si>
+    <t>Privacy roles and responsibilities are coordinated and aligned with third-party stakeholders (e.g., service providers, customers, partners).</t>
+  </si>
+  <si>
+    <t>GV_P.PP_P.P5</t>
+  </si>
+  <si>
+    <t>GV.PP-P5</t>
+  </si>
+  <si>
+    <t>Legal, regulatory, and contractual requirements regarding privacy are understood and managed.</t>
+  </si>
+  <si>
+    <t>6.15.1.1;5.2.1</t>
+  </si>
+  <si>
+    <t>GV_P.PP_P.P6</t>
+  </si>
+  <si>
+    <t>GV.PP-P6</t>
+  </si>
+  <si>
+    <t>Governance and risk management policies, processes and procedures address privacy risks.</t>
+  </si>
+  <si>
+    <t>GV_P.RM_P</t>
+  </si>
+  <si>
+    <t>GV.RM-P</t>
+  </si>
+  <si>
+    <t>Risk Management Strategy: The organization’s priorities, constraints, risk tolerances, and assumptions are established and used to support operational risk decisions.</t>
+  </si>
+  <si>
+    <t>GV_P.RM_P.P1</t>
+  </si>
+  <si>
+    <t>GV.RM-P1</t>
+  </si>
+  <si>
+    <t>Risk management processes are established, managed, and agreed to by organizational stakeholders.</t>
+  </si>
+  <si>
+    <t>GV_P.RM_P.P2</t>
+  </si>
+  <si>
+    <t>GV.RM-P2</t>
+  </si>
+  <si>
+    <t>Organizational risk tolerance is determined and clearly expressed.</t>
+  </si>
+  <si>
+    <t>5.4.1.2;5.4.1.3;5.2.4</t>
+  </si>
+  <si>
+    <t>GV_P.RM_P.P3</t>
+  </si>
+  <si>
+    <t>GV.RM-P3</t>
+  </si>
+  <si>
+    <t>The organization’s determination of risk tolerance is informed by its role in the data processing ecosystem.</t>
+  </si>
+  <si>
+    <t>GV_P.AT_P</t>
+  </si>
+  <si>
+    <t>GV.AT-P</t>
+  </si>
+  <si>
+    <t>Awareness and Training: The organization’s workforce and third parties engaged in data processing are provided privacy awareness education and are trained to perform their privacyrelated duties and responsibilities consistent with related policies, processes, procedures, and agreements and organizational privacy values.</t>
+  </si>
+  <si>
+    <t>GV_P.AT_P.P1</t>
+  </si>
+  <si>
+    <t>GV.AT-P1</t>
+  </si>
+  <si>
+    <t>The workforce is informed and trained on its roles and responsibilities.</t>
+  </si>
+  <si>
+    <t>GV_P.AT_P.P2</t>
+  </si>
+  <si>
+    <t>GV.AT-P2</t>
+  </si>
+  <si>
+    <t>Senior executives understand their roles and responsibilities.</t>
+  </si>
+  <si>
+    <t>GV_P.AT_P.P3</t>
+  </si>
+  <si>
+    <t>GV.AT-P3</t>
+  </si>
+  <si>
+    <t>Privacy personnel understand their roles and responsibilities.</t>
+  </si>
+  <si>
+    <t>GV_P.AT_P.P4</t>
+  </si>
+  <si>
+    <t>GV.AT-P4</t>
+  </si>
+  <si>
+    <t>Third parties (e.g., service providers, customers, partners) understand their roles and responsibilities.</t>
+  </si>
+  <si>
+    <t>6.12.1.2;6.2.1.1;7.2.6;8.2.1;8.2.4;7.3.3;8.3.1</t>
+  </si>
+  <si>
+    <t>GV_P.MT_P</t>
+  </si>
+  <si>
+    <t>GV.MT-P</t>
+  </si>
+  <si>
+    <t>Monitoring and Review: The policies, processes, and procedures for ongoing review of the organization’s privacy posture are understood and inform the management of privacy risk.</t>
+  </si>
+  <si>
+    <t>GV_P.MT_P.P1</t>
+  </si>
+  <si>
+    <t>GV.MT-P1</t>
+  </si>
+  <si>
+    <t>Privacy risk is re-evaluated on an ongoing basis and as key factors, including the organization’s business environment, governance (e.g., legal obligations, risk tolerance), data processing, and systems/products/services change.</t>
+  </si>
+  <si>
+    <t>GV_P.MT_P.P2</t>
+  </si>
+  <si>
+    <t>GV.MT-P2</t>
+  </si>
+  <si>
+    <t>Privacy values, policies, and training are reviewed and any updates are communicated.</t>
+  </si>
+  <si>
+    <t>6.2.1.1;6.3.1.1</t>
+  </si>
+  <si>
+    <t>GV_P.MT_P.P3</t>
+  </si>
+  <si>
+    <t>GV.MT-P3</t>
+  </si>
+  <si>
+    <t>Policies, processes, and procedures for assessing compliance with legal requirements and privacy policies are established and in place.</t>
+  </si>
+  <si>
+    <t>GV_P.MT_P.P4</t>
+  </si>
+  <si>
+    <t>GV.MT-P4</t>
+  </si>
+  <si>
+    <t>Policies, processes, and procedures for communicating progress on managing privacy risks are established and in place.</t>
+  </si>
+  <si>
+    <t>GV_P.MT_P.P5</t>
+  </si>
+  <si>
+    <t>GV.MT-P5</t>
+  </si>
+  <si>
+    <t>Policies, processes, and procedures are established and in place to receive, analyze, and respond to problematic data actions disclosed to the organization from internal and external sources (e.g., internal discovery, privacy researchers).</t>
+  </si>
+  <si>
+    <t>6.13.1.2;6.13.1.3</t>
+  </si>
+  <si>
+    <t>GV_P.MT_P.P6</t>
+  </si>
+  <si>
+    <t>GV.MT-P6</t>
+  </si>
+  <si>
+    <t>Policies, processes, and procedures incorporate lessons learned from problematic data actions.</t>
+  </si>
+  <si>
+    <t>GV_P.MT_P.P7</t>
+  </si>
+  <si>
+    <t>GV.MT-P7</t>
+  </si>
+  <si>
+    <t>Policies, processes, and procedures for receiving, tracking, and responding to complaints, concerns, and questions from individuals about organizational privacy practices are established and in place.</t>
+  </si>
+  <si>
+    <t>7.3.9;8.3.1</t>
+  </si>
+  <si>
+    <t>CT_P</t>
+  </si>
+  <si>
+    <t>CT-P</t>
+  </si>
+  <si>
+    <t>CONTROL-P: Develop and implement appropriate activities to enable organizations or individuals to manage data with</t>
+  </si>
+  <si>
+    <t>CT_P.PO_P</t>
+  </si>
+  <si>
+    <t>CT.PO-P</t>
+  </si>
+  <si>
+    <t>Data Management Policies, Processes, and Procedures: Policies, processes, and procedures are maintained and used to</t>
+  </si>
+  <si>
+    <t>CT_P.PO_P.P1</t>
+  </si>
+  <si>
+    <t>CT.PO-P1</t>
+  </si>
+  <si>
+    <t>Policies, processes, and procedures for authorizing data processing (e.g., organizational decisions, individual consent), revoking authorizations, and maintaining authorizations are established and in place.</t>
+  </si>
+  <si>
+    <t>CT_P.PO_P.P2</t>
+  </si>
+  <si>
+    <t>CT.PO-P2</t>
+  </si>
+  <si>
+    <t>Policies, processes, and procedures for enabling data review, transfer, sharing or disclosure, alteration, and deletion are established and in place.</t>
+  </si>
+  <si>
+    <t>7.3.1;7.3.4;7.3.5;7.3.6;7.3.8;7.3.10;7.5.1;7.5.2;7.5.3;7.5.4;8.3.1;8.5.1;8.5.2;8.5.3;8.5.4;8.5.5;8.5.6;8.5.7;8.5.8</t>
+  </si>
+  <si>
+    <t>CT_P.PO_P.P3</t>
+  </si>
+  <si>
+    <t>CT.PO-P3</t>
+  </si>
+  <si>
+    <t>Policies, processes, and procedures for enabling individuals’ data processing preferences and requests are established and in place.</t>
+  </si>
+  <si>
+    <t>7.3.1;7.3.4;7.3.5;7.3.6;7.3.8;7.3.10;8.3.1</t>
+  </si>
+  <si>
+    <t>CT_P.PO_P.P4</t>
+  </si>
+  <si>
+    <t>CT.PO-P4</t>
+  </si>
+  <si>
+    <t>An information life cycle to manage data is aligned and implemented with the system development life cycle to manage systems.</t>
+  </si>
+  <si>
+    <t>CT_P.DM_P</t>
+  </si>
+  <si>
+    <t>CT.DM-P</t>
+  </si>
+  <si>
+    <t>Data Management: Data are managed consistent with the organization’s risk strategy to protect individuals’ privacy, increase manageability, and enable the implementation of privacy principles (e.g., individual participation, data quality, data minimization).</t>
+  </si>
+  <si>
+    <t>CT_P.DM_P.P1</t>
+  </si>
+  <si>
+    <t>CT.DM-P1</t>
+  </si>
+  <si>
+    <t>Data elements can be accessed for review.</t>
+  </si>
+  <si>
+    <t>CT_P.DM_P.P2</t>
+  </si>
+  <si>
+    <t>CT.DM-P2</t>
+  </si>
+  <si>
+    <t>Data elements can be accessed for transmission or disclosure.</t>
+  </si>
+  <si>
+    <t>CT_P.DM_P.P3</t>
+  </si>
+  <si>
+    <t>CT.DM-P3</t>
+  </si>
+  <si>
+    <t>Data elements can be accessed for alteration.</t>
+  </si>
+  <si>
+    <t>CT_P.DM_P.P4</t>
+  </si>
+  <si>
+    <t>CT.DM-P4</t>
+  </si>
+  <si>
+    <t>Data elements can be accessed for deletion.</t>
+  </si>
+  <si>
+    <t>CT_P.DM_P.P5</t>
+  </si>
+  <si>
+    <t>CT.DM-P5</t>
+  </si>
+  <si>
+    <t>Data are destroyed according to policy.</t>
+  </si>
+  <si>
+    <t>7.4.8;7.4.5</t>
+  </si>
+  <si>
+    <t>CT_P.DM_P.P6</t>
+  </si>
+  <si>
+    <t>CT.DM-P6</t>
+  </si>
+  <si>
+    <t>Data are transmitted using standardized formats.</t>
+  </si>
+  <si>
+    <t>CT_P.DM_P.P7</t>
+  </si>
+  <si>
+    <t>CT.DM-P7</t>
+  </si>
+  <si>
+    <t>Metadata containing processing permissions and related data values are transmitted with data elements.</t>
+  </si>
+  <si>
+    <t>6.5.3.2;6.8.2.7;7.4.8;7.4.6;7.4.7;8.4.1;8.4.2</t>
+  </si>
+  <si>
+    <t>CT_P.DM_P.P8</t>
+  </si>
+  <si>
+    <t>CT.DM-P8</t>
+  </si>
+  <si>
+    <t>Audit/log records are determined, documented, implemented, and reviewed in accordance with policy and incorporating the principle of data minimization.</t>
+  </si>
+  <si>
+    <t>6.9.4.1;6.9.4.2;6.15.1.3</t>
+  </si>
+  <si>
+    <t>CT_P.DP_P</t>
+  </si>
+  <si>
+    <t>CT.DP-P</t>
+  </si>
+  <si>
+    <t>Disassociated Processing: Data processing solutions increase</t>
+  </si>
+  <si>
+    <t>CT_P.DP_P.P1</t>
+  </si>
+  <si>
+    <t>CT.DP-P1</t>
+  </si>
+  <si>
+    <t>Data are processed in an unobservable or unlinkable manner (e.g., data actions take place on local devices, privacy-preserving cryptography).</t>
+  </si>
+  <si>
+    <t>CT_P.DP_P.P2</t>
+  </si>
+  <si>
+    <t>CT.DP-P2</t>
+  </si>
+  <si>
+    <t>Data are processed to limit the identification of individuals (e.g., differential privacy techniques, tokenization).</t>
+  </si>
+  <si>
+    <t>7.4.2;7.4.4</t>
+  </si>
+  <si>
+    <t>CT_P.DP_P.P3</t>
+  </si>
+  <si>
+    <t>CT.DP-P3</t>
+  </si>
+  <si>
+    <t>Data are processed to restrict the formulation of inferences about individuals’ behavior or activities (e.g., data processing is decentralized, distributed architectures).</t>
+  </si>
+  <si>
+    <t>7.4.2;8.2.2;8.2.3;8.2.4</t>
+  </si>
+  <si>
+    <t>CT_P.DP_P.P4</t>
+  </si>
+  <si>
+    <t>CT.DP-P4</t>
+  </si>
+  <si>
+    <t>System or device configurations permit selective collection or disclosure of data elements.</t>
+  </si>
+  <si>
+    <t>CT_P.DP_P.P5</t>
+  </si>
+  <si>
+    <t>CT.DP-P5</t>
+  </si>
+  <si>
+    <t>Attribute references are substituted for attribute values.</t>
+  </si>
+  <si>
+    <t>CT_P.DP_P.P6</t>
+  </si>
+  <si>
+    <t>CT.DP-P6</t>
+  </si>
+  <si>
+    <t>Data processing is limited to that which is relevant and necessary for a system/product/service to meet mission/business objectives.</t>
+  </si>
+  <si>
+    <t>CM_P</t>
+  </si>
+  <si>
+    <t>CM-P</t>
+  </si>
+  <si>
+    <t>COMMUNICATE-P: Develop and implement appropriate activities to enable organizations and individuals to have a reliable understanding about how data are processed and associated privacy risks.</t>
+  </si>
+  <si>
+    <t>CM_P.PP_P</t>
+  </si>
+  <si>
+    <t>CM.PP-P</t>
+  </si>
+  <si>
+    <t>Communication Policies, Processes, and Procedures: Policies, processes, and procedures are maintained and used to increase transparency of the organization’s data processing practices (e.g., purpose, scope, roles, responsibilities, management commitment, and coordination among organizational entities) and associated privacy risks</t>
+  </si>
+  <si>
+    <t>CM_P.PP_P.P1</t>
+  </si>
+  <si>
+    <t>CM.PP-P1</t>
+  </si>
+  <si>
+    <t>Transparency policies, processes, and procedures for communicating data processing purposes, practices, and associated privacy risks are established and in place.</t>
+  </si>
+  <si>
+    <t>7.3.2;7.3.3;8.3.1</t>
+  </si>
+  <si>
+    <t>CM_P.PP_P.P2</t>
+  </si>
+  <si>
+    <t>CM.PP-P2</t>
+  </si>
+  <si>
+    <t>Roles and responsibilities (e.g., public relations) for communicating data processing purposes, practices, and associated privacy risks are established.</t>
+  </si>
+  <si>
+    <t>6.3.1.1;7.3.2;7.3.3;8.3.1</t>
+  </si>
+  <si>
+    <t>CM_P.AW_P</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CM.AW-P</t>
+  </si>
+  <si>
+    <t>Data Processing Awareness: Individuals and organizations have reliable knowledge about data processing practices and associated privacy risks, and effective mechanisms are used and maintained to increase predictability consistent with the organization’s risk strategy to protect individuals’ privacy.</t>
+  </si>
+  <si>
+    <t>CM_P.AW_P.P1</t>
+  </si>
+  <si>
+    <t>CM.AW-P1</t>
+  </si>
+  <si>
+    <t>Mechanisms (e.g., notices, internal or public reports) for communicating data processing purposes, practices, associated privacy risks, and options for enabling individuals’ data processing preferences and requests are established and in place.</t>
+  </si>
+  <si>
+    <t>CM_P.AW_P.P2</t>
+  </si>
+  <si>
+    <t>CM.AW-P2</t>
+  </si>
+  <si>
+    <t>Mechanisms for obtaining feedback from individuals (e.g., surveys or focus groups) about data processing and associated privacy risks are established and in place.</t>
+  </si>
+  <si>
+    <t>5.2.2;7.3.9;8.3.1</t>
+  </si>
+  <si>
+    <t>CM_P.AW_P.P3</t>
+  </si>
+  <si>
+    <t>CM.AW-P3</t>
+  </si>
+  <si>
+    <t>System/product/service design enables data processing visibility.</t>
+  </si>
+  <si>
+    <t>CM_P.AW_P.P4</t>
+  </si>
+  <si>
+    <t>CM.AW-P4</t>
+  </si>
+  <si>
+    <t>Records of data disclosures and sharing are maintained and can be accessed for review or transmission/disclosure.</t>
+  </si>
+  <si>
+    <t>7.5.4;8.5.3;8.5.4;8.5.5</t>
+  </si>
+  <si>
+    <t>CM_P.AW_P.P5</t>
+  </si>
+  <si>
+    <t>CM.AW-P5</t>
+  </si>
+  <si>
+    <t>Data corrections or deletions can be communicated to individuals or organizations (e.g., data sources) in the data processing ecosystem.</t>
+  </si>
+  <si>
+    <t>7.3.2;7.3.3;7.3.7;8.3.1</t>
+  </si>
+  <si>
+    <t>CM_P.AW_P.P6</t>
+  </si>
+  <si>
+    <t>CM.AW-P6</t>
+  </si>
+  <si>
+    <t>Data provenance and lineage are maintained and can be accessed for review or transmission/disclosure.</t>
+  </si>
+  <si>
+    <t>7.2.8;8.2.6;6.5.2.1;6.5.2.2</t>
+  </si>
+  <si>
+    <t>CM_P.AW_P.P7</t>
+  </si>
+  <si>
+    <t>CM.AW-P7</t>
+  </si>
+  <si>
+    <t>Impacted individuals and organizations are notified about a privacy breach or event.</t>
+  </si>
+  <si>
+    <t>CM_P.AW_P.P8</t>
+  </si>
+  <si>
+    <t>CM.AW-P8</t>
+  </si>
+  <si>
+    <t>Individuals are provided with mitigation mechanisms to address impacts to individuals that arise from data processing.</t>
+  </si>
+  <si>
+    <t>PR_P</t>
+  </si>
+  <si>
+    <t>PR-P</t>
+  </si>
+  <si>
+    <t>PROTECT-P: Develop and implement appropriate data processing safeguards</t>
+  </si>
+  <si>
+    <t>PR_P.AC_P</t>
+  </si>
+  <si>
+    <t>PR.AC-P</t>
+  </si>
+  <si>
+    <t>Identity Management, Authentication, and Access Control (PR.AC-P): Access to data and devices is limited to authorized individuals,processes, and devices, and is managed consistent with the assessed risk of unauthorized access.</t>
+  </si>
+  <si>
+    <t>PR_P.AC_P.P1</t>
+  </si>
+  <si>
+    <t>PR.AC-P1</t>
+  </si>
+  <si>
+    <t>Identities and credentials are issued, managed, verified, revoked, and audited for authorized individuals, processes, and devices</t>
+  </si>
+  <si>
+    <t>6.6.2.1;6.6.2.2;6.6.4.2</t>
+  </si>
+  <si>
+    <t>PR_P.AC_P.P2</t>
+  </si>
+  <si>
+    <t>PR.AC-P2</t>
+  </si>
+  <si>
+    <t>Physical access to data and devices is managed.</t>
+  </si>
+  <si>
+    <t>6.6.2.1;6.6.2.2;6.3.2.1</t>
+  </si>
+  <si>
+    <t>PR_P.AC_P.P3</t>
+  </si>
+  <si>
+    <t>PR.AC-P3</t>
+  </si>
+  <si>
+    <t>Remote access is managed.</t>
+  </si>
+  <si>
+    <t>6.6.2.1;6.6.2.2</t>
+  </si>
+  <si>
+    <t>PR_P.AC_P.P4</t>
+  </si>
+  <si>
+    <t>PR.AC-P4</t>
+  </si>
+  <si>
+    <t>Access permissions and authorizations are managed, incorporating the principles of least privilege and separation of duties.</t>
+  </si>
+  <si>
+    <t>PR_P.AC_P.P5</t>
+  </si>
+  <si>
+    <t>PR.AC-P5</t>
+  </si>
+  <si>
+    <t>Network integrity is protected (e.g., network segregation, network segmentation).</t>
+  </si>
+  <si>
+    <t>PR_P.AC_P.P6</t>
+  </si>
+  <si>
+    <t>PR.AC-P6</t>
+  </si>
+  <si>
+    <t>Individuals and devices are proofed and bound to credentials, and authenticated commensurate with the risk of the transaction (e.g., individuals’ security and privacy risks and other organizational risks).</t>
+  </si>
+  <si>
+    <t>PR_P.DS_P</t>
+  </si>
+  <si>
+    <t>PR.DS-P</t>
+  </si>
+  <si>
+    <t>Data Security: Data are managed consistent with the organization’s risk strategy to protect individuals’ privacy and maintain data confidentiality, integrity, and availability.</t>
+  </si>
+  <si>
+    <t>PR_P.DS_P.P1</t>
+  </si>
+  <si>
+    <t>PR.DS-P1</t>
+  </si>
+  <si>
+    <t>Data-at-rest are protected</t>
+  </si>
+  <si>
+    <t>PR_P.DS_P.P2</t>
+  </si>
+  <si>
+    <t>PR.DS-P2</t>
+  </si>
+  <si>
+    <t>Data-in-transit are protected.</t>
+  </si>
+  <si>
+    <t>6.5.3.3;6.11.1.2</t>
+  </si>
+  <si>
+    <t>PR_P.DS_P.P3</t>
+  </si>
+  <si>
+    <t>PR.DS-P3</t>
+  </si>
+  <si>
+    <t>Systems/products/services and associated data are formally managed throughout removal, transfers, and disposition.</t>
+  </si>
+  <si>
+    <t>6.5.3.2;6.8.2.7;7.4.5;7.4.6;7.4.8;7.4.9;8.4.2</t>
+  </si>
+  <si>
+    <t>PR_P.DS_P.P4</t>
+  </si>
+  <si>
+    <t>PR.DS-P4</t>
+  </si>
+  <si>
+    <t>Adequate capacity to ensure availability is maintained.</t>
+  </si>
+  <si>
+    <t>PR_P.DS_P.P5</t>
+  </si>
+  <si>
+    <t>PR.DS-P5</t>
+  </si>
+  <si>
+    <t>Protections against data leaks are implemented.</t>
+  </si>
+  <si>
+    <t>6.5.3.2;6.8.2.1;6.11.2.4;6.10.2.4</t>
+  </si>
+  <si>
+    <t>PR_P.DS_P.P6</t>
+  </si>
+  <si>
+    <t>PR.DS-P6</t>
+  </si>
+  <si>
+    <t>Integrity checking mechanisms are used to verify software, firmware, and information integrity.</t>
+  </si>
+  <si>
+    <t>PR_P.DS_P.P7</t>
+  </si>
+  <si>
+    <t>PR.DS-P7</t>
+  </si>
+  <si>
+    <t>The development and testing environment(s) are separate from the production environment.</t>
+  </si>
+  <si>
+    <t>PR_P.DS_P.P8</t>
+  </si>
+  <si>
+    <t>PR.DS-P8</t>
+  </si>
+  <si>
+    <t>Integrity checking mechanisms are used to verify hardware integrity.</t>
+  </si>
+  <si>
+    <t>PR_P.DP_P</t>
+  </si>
+  <si>
+    <t>PR.DP-P</t>
+  </si>
+  <si>
+    <t>Data Protection Policies, Processes, and Procedures: Security and privacy policies (which address purpose, scope, roles, responsibilities, management commitment, and coordination among organizational entities), processes, and procedures are maintained and used to manage the protection of data.</t>
+  </si>
+  <si>
+    <t>PR_P.DP_P.P1</t>
+  </si>
+  <si>
+    <t>PR.DP-P1</t>
+  </si>
+  <si>
+    <t>A baseline configuration of information technology is created and maintained incorporating security principles (e.g., concept of least functionality).</t>
+  </si>
+  <si>
+    <t>PR_P.DP_P.P2</t>
+  </si>
+  <si>
+    <t>PR.DP-P2</t>
+  </si>
+  <si>
+    <t>Configuration change control processes are established and in place.</t>
+  </si>
+  <si>
+    <t>PR_P.DP_P.P3</t>
+  </si>
+  <si>
+    <t>PR.DP-P3</t>
+  </si>
+  <si>
+    <t>Backups of information are conducted, maintained, and tested.</t>
+  </si>
+  <si>
+    <t>PR_P.DP_P.P4</t>
+  </si>
+  <si>
+    <t>PR.DP-P4</t>
+  </si>
+  <si>
+    <t>Policy and regulations regarding the physical operating environment for organizational assets are met.</t>
+  </si>
+  <si>
+    <t>PR_P.DP_P.P5</t>
+  </si>
+  <si>
+    <t>PR.DP-P5</t>
+  </si>
+  <si>
+    <t>Protection processes are improved.</t>
+  </si>
+  <si>
+    <t>PR_P.DP_P.P6</t>
+  </si>
+  <si>
+    <t>PR.DP-P6</t>
+  </si>
+  <si>
+    <t>Effectiveness of protection technologies is shared.</t>
+  </si>
+  <si>
+    <t>7.3.3;8.3.1</t>
+  </si>
+  <si>
+    <t>PR_P.DP_P.P7</t>
+  </si>
+  <si>
+    <t>PR.DP-P7</t>
+  </si>
+  <si>
+    <t>Response plans (Incident Response and Business Continuity) and recovery plans (Incident Recovery and Disaster Recovery) are established, in place, and managed.</t>
+  </si>
+  <si>
+    <t>6.13.1.1;6.14.1.1</t>
+  </si>
+  <si>
+    <t>PR_P.DP_P.P8</t>
+  </si>
+  <si>
+    <t>PR.DP-P8</t>
+  </si>
+  <si>
+    <t>Response and recovery plans are tested.</t>
+  </si>
+  <si>
+    <t>PR_P.DP_P.P9</t>
+  </si>
+  <si>
+    <t>PR.DP-P9</t>
+  </si>
+  <si>
+    <t>Privacy procedures are included in human resources practices (e.g., deprovisioning, personnel screening).</t>
+  </si>
+  <si>
+    <t>6.10.2.4;6.6.2.2;6.8.2.9</t>
+  </si>
+  <si>
+    <t>PR_P.DP_P.P10</t>
+  </si>
+  <si>
+    <t>PR.DP-P10</t>
+  </si>
+  <si>
+    <t>A vulnerability management plan is developed and implemented.</t>
+  </si>
+  <si>
+    <t>PR_P.MA_P</t>
+  </si>
+  <si>
+    <t>PR.MA-P</t>
+  </si>
+  <si>
+    <t>Maintenance: System maintenance and repairs are performed consistent with policies, processes, and procedures.</t>
+  </si>
+  <si>
+    <t>PR_P.MA_P.P1</t>
+  </si>
+  <si>
+    <t>PR.MA-P1</t>
+  </si>
+  <si>
+    <t>Maintenance and repair of organizational assets are performed and logged, with approved and controlled tools.</t>
+  </si>
+  <si>
+    <t>PR_P.MA_P.P2</t>
+  </si>
+  <si>
+    <t>PR.MA-P2</t>
+  </si>
+  <si>
+    <t>Remote maintenance of organizational assets is approved, logged, and performed in a manner that prevents unauthorized access.</t>
+  </si>
+  <si>
+    <t>PR_P.PT_P</t>
+  </si>
+  <si>
+    <t>PR.PT-P</t>
+  </si>
+  <si>
+    <t>Protective Technology: Technical security solutions are managed to ensure the security and resilience of systems/products/services and associated data, consistent with related policies, processes, procedures, and agreements.</t>
+  </si>
+  <si>
+    <t>PR_P.PT_P.P1</t>
+  </si>
+  <si>
+    <t>PR.PT-P1</t>
+  </si>
+  <si>
+    <t>Removable media is protected and its use restricted according to policy.</t>
+  </si>
+  <si>
+    <t>6.5.3.1;6.5.3.2</t>
+  </si>
+  <si>
+    <t>PR_P.PT_P.P2</t>
+  </si>
+  <si>
+    <t>PR.PT-P2</t>
+  </si>
+  <si>
+    <t>The principle of least functionality is incorporated by configuring systems to provide only essential capabilities.</t>
+  </si>
+  <si>
+    <t>PR_P.PT_P.P3</t>
+  </si>
+  <si>
+    <t>PR.PT-P3</t>
+  </si>
+  <si>
+    <t>Communications and control networks are protected.</t>
+  </si>
+  <si>
+    <t>6.10.1.1;6.10.1.2;6.10.1.3;6.10.2.1</t>
+  </si>
+  <si>
+    <t>PR_P.PT_P.P4</t>
+  </si>
+  <si>
+    <t>PR.PT-P4</t>
+  </si>
+  <si>
+    <t>Mechanisms (e.g., failsafe, load balancing, hot swap) are implemented to achieve resilience requirements in normal and adverse situations.</t>
   </si>
 </sst>
 </file>
@@ -16860,6 +18076,1685 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F381F253-97F6-4162-AAC0-64DEB2D11E21}">
+  <dimension ref="A1:E123"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="62.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30">
+      <c r="A2" t="s">
+        <v>2808</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2809</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2810</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30">
+      <c r="A3" t="s">
+        <v>2811</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2812</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2813</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>2814</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2815</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2816</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="75">
+      <c r="A5" t="s">
+        <v>2817</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2818</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>2819</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>2820</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45">
+      <c r="A6" t="s">
+        <v>2821</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2822</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>2823</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>2824</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2825</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>2826</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>2827</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2828</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>2829</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>2830</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>2831</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2832</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>2833</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>2834</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30">
+      <c r="A10" t="s">
+        <v>2835</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2836</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>2837</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>2838</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="75">
+      <c r="A11" t="s">
+        <v>2839</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2840</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>2841</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>2838</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="60">
+      <c r="A12" t="s">
+        <v>2842</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2843</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>2844</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30">
+      <c r="A13" t="s">
+        <v>2845</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2846</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>2847</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>2848</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30">
+      <c r="A14" t="s">
+        <v>2849</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2850</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>2851</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30">
+      <c r="A15" t="s">
+        <v>2852</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2853</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>2854</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>2855</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="75">
+      <c r="A16" t="s">
+        <v>2856</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2857</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>2858</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="60">
+      <c r="A17" t="s">
+        <v>2859</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2860</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>2861</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>2806</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30">
+      <c r="A18" t="s">
+        <v>2862</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2863</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>2864</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>2865</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30">
+      <c r="A19" t="s">
+        <v>2866</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2867</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>2868</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30">
+      <c r="A20" t="s">
+        <v>2869</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2870</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>2871</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>2872</v>
+      </c>
+      <c r="B21" t="s">
+        <v>2873</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>2874</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>2875</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="105">
+      <c r="A22" t="s">
+        <v>2876</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2877</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>2878</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="45">
+      <c r="A23" t="s">
+        <v>2879</v>
+      </c>
+      <c r="B23" t="s">
+        <v>2880</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>2881</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="60">
+      <c r="A24" t="s">
+        <v>2882</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2883</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>2884</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="45">
+      <c r="A25" t="s">
+        <v>2885</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2886</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>2887</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>2888</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="30">
+      <c r="A26" t="s">
+        <v>2889</v>
+      </c>
+      <c r="B26" t="s">
+        <v>2890</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>2891</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="45">
+      <c r="A27" t="s">
+        <v>2892</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2893</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>2894</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="45">
+      <c r="A28" t="s">
+        <v>2895</v>
+      </c>
+      <c r="B28" t="s">
+        <v>2896</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>2897</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="60">
+      <c r="A29" t="s">
+        <v>2898</v>
+      </c>
+      <c r="B29" t="s">
+        <v>2899</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>2900</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="45">
+      <c r="A30" t="s">
+        <v>2901</v>
+      </c>
+      <c r="B30" t="s">
+        <v>2902</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>2903</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="45">
+      <c r="A31" t="s">
+        <v>2904</v>
+      </c>
+      <c r="B31" t="s">
+        <v>2905</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>2906</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="30">
+      <c r="A32" t="s">
+        <v>2907</v>
+      </c>
+      <c r="B32" t="s">
+        <v>2908</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>2909</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="45">
+      <c r="A33" t="s">
+        <v>2910</v>
+      </c>
+      <c r="B33" t="s">
+        <v>2911</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>2912</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="30">
+      <c r="A34" t="s">
+        <v>2913</v>
+      </c>
+      <c r="B34" t="s">
+        <v>2914</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>2915</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>2916</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="30">
+      <c r="A35" t="s">
+        <v>2917</v>
+      </c>
+      <c r="B35" t="s">
+        <v>2918</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>2919</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>2875</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="45">
+      <c r="A36" t="s">
+        <v>2920</v>
+      </c>
+      <c r="B36" t="s">
+        <v>2921</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>2922</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="30">
+      <c r="A37" t="s">
+        <v>2923</v>
+      </c>
+      <c r="B37" t="s">
+        <v>2924</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>2925</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>2875</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>2926</v>
+      </c>
+      <c r="B38" t="s">
+        <v>2927</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>2928</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>2929</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="30">
+      <c r="A39" t="s">
+        <v>2930</v>
+      </c>
+      <c r="B39" t="s">
+        <v>2931</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>2932</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>2875</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="75">
+      <c r="A40" t="s">
+        <v>2933</v>
+      </c>
+      <c r="B40" t="s">
+        <v>2934</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>2935</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="30">
+      <c r="A41" t="s">
+        <v>2936</v>
+      </c>
+      <c r="B41" t="s">
+        <v>2937</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>2938</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>2939</v>
+      </c>
+      <c r="B42" t="s">
+        <v>2940</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>2941</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>2942</v>
+      </c>
+      <c r="B43" t="s">
+        <v>2943</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>2944</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="30">
+      <c r="A44" t="s">
+        <v>2945</v>
+      </c>
+      <c r="B44" t="s">
+        <v>2946</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>2947</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>2948</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="45">
+      <c r="A45" t="s">
+        <v>2949</v>
+      </c>
+      <c r="B45" t="s">
+        <v>2950</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>2951</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="60">
+      <c r="A46" t="s">
+        <v>2952</v>
+      </c>
+      <c r="B46" t="s">
+        <v>2953</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>2954</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="30">
+      <c r="A47" t="s">
+        <v>2955</v>
+      </c>
+      <c r="B47" t="s">
+        <v>2956</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>2957</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>2958</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="45">
+      <c r="A48" t="s">
+        <v>2959</v>
+      </c>
+      <c r="B48" t="s">
+        <v>2960</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>2961</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="30">
+      <c r="A49" t="s">
+        <v>2962</v>
+      </c>
+      <c r="B49" t="s">
+        <v>2963</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>2964</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="60">
+      <c r="A50" t="s">
+        <v>2965</v>
+      </c>
+      <c r="B50" t="s">
+        <v>2966</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>2967</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>2968</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="30">
+      <c r="A51" t="s">
+        <v>2969</v>
+      </c>
+      <c r="B51" t="s">
+        <v>2970</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>2971</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="60">
+      <c r="A52" t="s">
+        <v>2972</v>
+      </c>
+      <c r="B52" t="s">
+        <v>2973</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>2974</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>2975</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="30">
+      <c r="A53" t="s">
+        <v>2976</v>
+      </c>
+      <c r="B53" t="s">
+        <v>2977</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>2978</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="30">
+      <c r="A54" t="s">
+        <v>2979</v>
+      </c>
+      <c r="B54" t="s">
+        <v>2980</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>2981</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="60">
+      <c r="A55" t="s">
+        <v>2982</v>
+      </c>
+      <c r="B55" t="s">
+        <v>2983</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>2984</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>2787</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="75">
+      <c r="A56" t="s">
+        <v>2985</v>
+      </c>
+      <c r="B56" t="s">
+        <v>2986</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>2987</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>2988</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="30">
+      <c r="A57" t="s">
+        <v>2989</v>
+      </c>
+      <c r="B57" t="s">
+        <v>2990</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>2991</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>2992</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="45">
+      <c r="A58" t="s">
+        <v>2993</v>
+      </c>
+      <c r="B58" t="s">
+        <v>2994</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>2995</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="75">
+      <c r="A59" t="s">
+        <v>2996</v>
+      </c>
+      <c r="B59" t="s">
+        <v>2997</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>2998</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>2999</v>
+      </c>
+      <c r="B60" t="s">
+        <v>3000</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>3001</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>3002</v>
+      </c>
+      <c r="B61" t="s">
+        <v>3003</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>3004</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>3005</v>
+      </c>
+      <c r="B62" t="s">
+        <v>3006</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>3007</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>3008</v>
+      </c>
+      <c r="B63" t="s">
+        <v>3009</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>3010</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>3011</v>
+      </c>
+      <c r="B64" t="s">
+        <v>3012</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>3013</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>3014</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>3015</v>
+      </c>
+      <c r="B65" t="s">
+        <v>3016</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>3017</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="30">
+      <c r="A66" t="s">
+        <v>3018</v>
+      </c>
+      <c r="B66" t="s">
+        <v>3019</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>3020</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>3021</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="45">
+      <c r="A67" t="s">
+        <v>3022</v>
+      </c>
+      <c r="B67" t="s">
+        <v>3023</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>3024</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>3025</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" t="s">
+        <v>3026</v>
+      </c>
+      <c r="B68" t="s">
+        <v>3027</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>3028</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="45">
+      <c r="A69" t="s">
+        <v>3029</v>
+      </c>
+      <c r="B69" t="s">
+        <v>3030</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>3031</v>
+      </c>
+      <c r="E69" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="30">
+      <c r="A70" t="s">
+        <v>3032</v>
+      </c>
+      <c r="B70" t="s">
+        <v>3033</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>3034</v>
+      </c>
+      <c r="E70" t="s">
+        <v>3035</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="45">
+      <c r="A71" t="s">
+        <v>3036</v>
+      </c>
+      <c r="B71" t="s">
+        <v>3037</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>3038</v>
+      </c>
+      <c r="E71" t="s">
+        <v>3039</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="30">
+      <c r="A72" t="s">
+        <v>3040</v>
+      </c>
+      <c r="B72" t="s">
+        <v>3041</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>3042</v>
+      </c>
+      <c r="E72" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" t="s">
+        <v>3043</v>
+      </c>
+      <c r="B73" t="s">
+        <v>3044</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>3045</v>
+      </c>
+      <c r="E73" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="30">
+      <c r="A74" t="s">
+        <v>3046</v>
+      </c>
+      <c r="B74" t="s">
+        <v>3047</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>3048</v>
+      </c>
+      <c r="E74" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="60">
+      <c r="A75" t="s">
+        <v>3049</v>
+      </c>
+      <c r="B75" t="s">
+        <v>3050</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>3051</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="90">
+      <c r="A76" t="s">
+        <v>3052</v>
+      </c>
+      <c r="B76" t="s">
+        <v>3053</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>3054</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="45">
+      <c r="A77" t="s">
+        <v>3055</v>
+      </c>
+      <c r="B77" t="s">
+        <v>3056</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>3057</v>
+      </c>
+      <c r="E77" t="s">
+        <v>3058</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="45">
+      <c r="A78" t="s">
+        <v>3059</v>
+      </c>
+      <c r="B78" t="s">
+        <v>3060</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>3061</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>3062</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="75">
+      <c r="A79" t="s">
+        <v>3063</v>
+      </c>
+      <c r="B79" t="s">
+        <v>3064</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>3065</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="60">
+      <c r="A80" t="s">
+        <v>3066</v>
+      </c>
+      <c r="B80" t="s">
+        <v>3067</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>3068</v>
+      </c>
+      <c r="E80" t="s">
+        <v>3058</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="45">
+      <c r="A81" t="s">
+        <v>3069</v>
+      </c>
+      <c r="B81" t="s">
+        <v>3070</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>3071</v>
+      </c>
+      <c r="E81" t="s">
+        <v>3072</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" t="s">
+        <v>3073</v>
+      </c>
+      <c r="B82" t="s">
+        <v>3074</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>3075</v>
+      </c>
+      <c r="E82" t="s">
+        <v>3058</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="30">
+      <c r="A83" t="s">
+        <v>3076</v>
+      </c>
+      <c r="B83" t="s">
+        <v>3077</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>3078</v>
+      </c>
+      <c r="E83" t="s">
+        <v>3079</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="45">
+      <c r="A84" t="s">
+        <v>3080</v>
+      </c>
+      <c r="B84" t="s">
+        <v>3081</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>3082</v>
+      </c>
+      <c r="E84" t="s">
+        <v>3083</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="30">
+      <c r="A85" t="s">
+        <v>3084</v>
+      </c>
+      <c r="B85" t="s">
+        <v>3085</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>3086</v>
+      </c>
+      <c r="E85" t="s">
+        <v>3087</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="30">
+      <c r="A86" t="s">
+        <v>3088</v>
+      </c>
+      <c r="B86" t="s">
+        <v>3089</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>3090</v>
+      </c>
+      <c r="E86" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="30">
+      <c r="A87" t="s">
+        <v>3091</v>
+      </c>
+      <c r="B87" t="s">
+        <v>3092</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>3093</v>
+      </c>
+      <c r="E87" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="30">
+      <c r="A88" t="s">
+        <v>3094</v>
+      </c>
+      <c r="B88" t="s">
+        <v>3095</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>3096</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="60">
+      <c r="A89" t="s">
+        <v>3097</v>
+      </c>
+      <c r="B89" t="s">
+        <v>3098</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>3099</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="30">
+      <c r="A90" t="s">
+        <v>3100</v>
+      </c>
+      <c r="B90" t="s">
+        <v>3101</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>3102</v>
+      </c>
+      <c r="E90" t="s">
+        <v>3103</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" t="s">
+        <v>3104</v>
+      </c>
+      <c r="B91" t="s">
+        <v>3105</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>3106</v>
+      </c>
+      <c r="E91" t="s">
+        <v>3107</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" t="s">
+        <v>3108</v>
+      </c>
+      <c r="B92" t="s">
+        <v>3109</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>3110</v>
+      </c>
+      <c r="E92" t="s">
+        <v>3111</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="30">
+      <c r="A93" t="s">
+        <v>3112</v>
+      </c>
+      <c r="B93" t="s">
+        <v>3113</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>3114</v>
+      </c>
+      <c r="E93" t="s">
+        <v>3111</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="30">
+      <c r="A94" t="s">
+        <v>3115</v>
+      </c>
+      <c r="B94" t="s">
+        <v>3116</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>3117</v>
+      </c>
+      <c r="E94" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="60">
+      <c r="A95" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B95" t="s">
+        <v>3119</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>3120</v>
+      </c>
+      <c r="E95" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="45">
+      <c r="A96" t="s">
+        <v>3121</v>
+      </c>
+      <c r="B96" t="s">
+        <v>3122</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>3123</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" t="s">
+        <v>3124</v>
+      </c>
+      <c r="B97" t="s">
+        <v>3125</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>3126</v>
+      </c>
+      <c r="E97" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" t="s">
+        <v>3127</v>
+      </c>
+      <c r="B98" t="s">
+        <v>3128</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>3129</v>
+      </c>
+      <c r="E98" t="s">
+        <v>3130</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="30">
+      <c r="A99" t="s">
+        <v>3131</v>
+      </c>
+      <c r="B99" t="s">
+        <v>3132</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>3133</v>
+      </c>
+      <c r="E99" t="s">
+        <v>3134</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" t="s">
+        <v>3135</v>
+      </c>
+      <c r="B100" t="s">
+        <v>3136</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>3137</v>
+      </c>
+      <c r="E100" t="s">
+        <v>1314</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="30">
+      <c r="A101" t="s">
+        <v>3138</v>
+      </c>
+      <c r="B101" t="s">
+        <v>3139</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>3140</v>
+      </c>
+      <c r="E101" s="3" t="s">
+        <v>3141</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="30">
+      <c r="A102" t="s">
+        <v>3142</v>
+      </c>
+      <c r="B102" t="s">
+        <v>3143</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>3144</v>
+      </c>
+      <c r="E102" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="30">
+      <c r="A103" t="s">
+        <v>3145</v>
+      </c>
+      <c r="B103" t="s">
+        <v>3146</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>3147</v>
+      </c>
+      <c r="E103" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="30">
+      <c r="A104" t="s">
+        <v>3148</v>
+      </c>
+      <c r="B104" t="s">
+        <v>3149</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>3150</v>
+      </c>
+      <c r="E104" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="75">
+      <c r="A105" t="s">
+        <v>3151</v>
+      </c>
+      <c r="B105" t="s">
+        <v>3152</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>3153</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="45">
+      <c r="A106" t="s">
+        <v>3154</v>
+      </c>
+      <c r="B106" t="s">
+        <v>3155</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>3156</v>
+      </c>
+      <c r="E106" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="30">
+      <c r="A107" t="s">
+        <v>3157</v>
+      </c>
+      <c r="B107" t="s">
+        <v>3158</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>3159</v>
+      </c>
+      <c r="E107" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" t="s">
+        <v>3160</v>
+      </c>
+      <c r="B108" t="s">
+        <v>3161</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>3162</v>
+      </c>
+      <c r="E108" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="30">
+      <c r="A109" t="s">
+        <v>3163</v>
+      </c>
+      <c r="B109" t="s">
+        <v>3164</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>3165</v>
+      </c>
+      <c r="E109">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
+      <c r="A110" t="s">
+        <v>3166</v>
+      </c>
+      <c r="B110" t="s">
+        <v>3167</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>3168</v>
+      </c>
+      <c r="E110" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
+      <c r="A111" t="s">
+        <v>3169</v>
+      </c>
+      <c r="B111" t="s">
+        <v>3170</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>3171</v>
+      </c>
+      <c r="E111" t="s">
+        <v>3172</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="45">
+      <c r="A112" t="s">
+        <v>3173</v>
+      </c>
+      <c r="B112" t="s">
+        <v>3174</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>3175</v>
+      </c>
+      <c r="E112" s="3" t="s">
+        <v>3176</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
+      <c r="A113" t="s">
+        <v>3177</v>
+      </c>
+      <c r="B113" t="s">
+        <v>3178</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>3179</v>
+      </c>
+      <c r="E113" t="s">
+        <v>1442</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="30">
+      <c r="A114" t="s">
+        <v>3180</v>
+      </c>
+      <c r="B114" t="s">
+        <v>3181</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>3182</v>
+      </c>
+      <c r="E114" t="s">
+        <v>3183</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="A115" t="s">
+        <v>3184</v>
+      </c>
+      <c r="B115" t="s">
+        <v>3185</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>3186</v>
+      </c>
+      <c r="E115" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="30">
+      <c r="A116" t="s">
+        <v>3187</v>
+      </c>
+      <c r="B116" t="s">
+        <v>3188</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>3189</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="30">
+      <c r="A117" t="s">
+        <v>3190</v>
+      </c>
+      <c r="B117" t="s">
+        <v>3191</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>3192</v>
+      </c>
+      <c r="E117" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="30">
+      <c r="A118" t="s">
+        <v>3193</v>
+      </c>
+      <c r="B118" t="s">
+        <v>3194</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>3195</v>
+      </c>
+      <c r="E118" t="s">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="60">
+      <c r="A119" t="s">
+        <v>3196</v>
+      </c>
+      <c r="B119" t="s">
+        <v>3197</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>3198</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
+      <c r="A120" t="s">
+        <v>3199</v>
+      </c>
+      <c r="B120" t="s">
+        <v>3200</v>
+      </c>
+      <c r="C120" t="s">
+        <v>3201</v>
+      </c>
+      <c r="E120" t="s">
+        <v>3202</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="30">
+      <c r="A121" t="s">
+        <v>3203</v>
+      </c>
+      <c r="B121" t="s">
+        <v>3204</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>3205</v>
+      </c>
+      <c r="E121" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="30">
+      <c r="A122" t="s">
+        <v>3206</v>
+      </c>
+      <c r="B122" t="s">
+        <v>3207</v>
+      </c>
+      <c r="C122" t="s">
+        <v>3208</v>
+      </c>
+      <c r="E122" s="3" t="s">
+        <v>3209</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="45">
+      <c r="A123" t="s">
+        <v>3210</v>
+      </c>
+      <c r="B123" t="s">
+        <v>3211</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>3212</v>
+      </c>
+      <c r="E123" t="s">
+        <v>1441</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G260"/>
@@ -21724,7 +24619,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24BA70E6-9548-4D87-8A65-060EC90D2814}">
   <dimension ref="A1:F664"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A318" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A318" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E328" sqref="E328"/>
     </sheetView>
   </sheetViews>
@@ -30354,6 +33249,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_STS_x0020_Hashtags xmlns="b38e6452-0983-483a-b0d4-324af6d44e4d"/>
+    <MediaServiceKeyPoints xmlns="b38e6452-0983-483a-b0d4-324af6d44e4d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010072B72D3E1CFCDD40BC0C6D9CCD45E0BB" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1091b63e79dc81a90741573e3164413c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="759c4387-f01d-437d-8a5d-56d9b05a6914" xmlns:ns4="b38e6452-0983-483a-b0d4-324af6d44e4d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7010e408eae2039b0bc4bac303a742c1" ns3:_="" ns4:_="">
     <xsd:import namespace="759c4387-f01d-437d-8a5d-56d9b05a6914"/>
@@ -30604,15 +33508,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_STS_x0020_Hashtags xmlns="b38e6452-0983-483a-b0d4-324af6d44e4d"/>
-    <MediaServiceKeyPoints xmlns="b38e6452-0983-483a-b0d4-324af6d44e4d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A59176D2-D324-41A5-A125-AC358C249804}">
   <ds:schemaRefs>
@@ -30622,6 +33517,16 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71725466-609F-438E-9D55-68B1CE9C392F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b38e6452-0983-483a-b0d4-324af6d44e4d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC11F96C-E600-42F3-BB18-A579B8C44705}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -30638,14 +33543,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71725466-609F-438E-9D55-68B1CE9C392F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b38e6452-0983-483a-b0d4-324af6d44e4d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
remove spacing in NIST mapping
</commit_message>
<xml_diff>
--- a/src/assets/database.xlsx
+++ b/src/assets/database.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16FBA2E4-7145-4633-B918-09AD688E5EA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{035AB369-DD7A-441C-B7DC-636F39FBAE7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8374,10 +8374,10 @@
     <t>Edited NIST Privacy Framework CT.DM-P5 to map to ISO 27701 7.4.5, 7.4.6, 7.4.8, 8.4.1, and 8.4.2. Also edited PR-DS-P5 to map to 6.2, 6.3, 6.4, 6.5, 6.6, 6.7, 6.8, 6.9, 6.10, 6.11, 6.12, 6.15</t>
   </si>
   <si>
-    <t>7.4.8;7.4.5; 7.4.6; 8.4.1;8.4.2</t>
-  </si>
-  <si>
     <t>6.2;6.3;6.4;6.5;6.6;6.7;6.8;6.9;6.10;6.11;6.12;6.15</t>
+  </si>
+  <si>
+    <t>7.4.8;7.4.5;7.4.6;8.4.1;8.4.2</t>
   </si>
 </sst>
 </file>
@@ -15011,8 +15011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D5AC0FA-9449-4B71-8884-9C6D19EE493B}">
   <dimension ref="A1:E123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E102" sqref="E102"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15881,7 +15881,7 @@
         <v>2255</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>2504</v>
+        <v>2505</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -16378,7 +16378,7 @@
         <v>2369</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>2505</v>
+        <v>2504</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -23274,21 +23274,21 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_STS_x0020_Hashtags xmlns="b38e6452-0983-483a-b0d4-324af6d44e4d"/>
+    <MediaServiceKeyPoints xmlns="b38e6452-0983-483a-b0d4-324af6d44e4d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_STS_x0020_Hashtags xmlns="b38e6452-0983-483a-b0d4-324af6d44e4d"/>
-    <MediaServiceKeyPoints xmlns="b38e6452-0983-483a-b0d4-324af6d44e4d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -23311,14 +23311,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A59176D2-D324-41A5-A125-AC358C249804}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71725466-609F-438E-9D55-68B1CE9C392F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -23326,4 +23318,12 @@
     <ds:schemaRef ds:uri="b38e6452-0983-483a-b0d4-324af6d44e4d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A59176D2-D324-41A5-A125-AC358C249804}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added spanish article 11 title for gdpr
</commit_message>
<xml_diff>
--- a/src/assets/database.xlsx
+++ b/src/assets/database.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1AC67E1-9DF7-412F-B7D5-D10E44A8AC8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58686069-8B69-4EDC-A163-6AC63B61AD39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7067" uniqueCount="3987">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7068" uniqueCount="3988">
   <si>
     <t>id</t>
   </si>
@@ -13364,6 +13364,9 @@
   </si>
   <si>
     <t>Added Spanish, Bulgarian, Finnish, and Swedish for GDPR; Reorder listing of regulations to be alphabetical</t>
+  </si>
+  <si>
+    <t>Tratamiento que no requiere identificación</t>
   </si>
 </sst>
 </file>
@@ -20294,9 +20297,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBB62EA1-5A3C-446A-BD82-9DFA95F5937C}">
   <dimension ref="A1:N406"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22217,7 +22220,9 @@
       <c r="H51" t="s">
         <v>669</v>
       </c>
-      <c r="I51" s="3"/>
+      <c r="I51" s="3" t="s">
+        <v>3987</v>
+      </c>
       <c r="J51" t="s">
         <v>669</v>
       </c>
@@ -37628,21 +37633,21 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_STS_x0020_Hashtags xmlns="b38e6452-0983-483a-b0d4-324af6d44e4d"/>
     <MediaServiceKeyPoints xmlns="b38e6452-0983-483a-b0d4-324af6d44e4d" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -37665,6 +37670,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A59176D2-D324-41A5-A125-AC358C249804}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71725466-609F-438E-9D55-68B1CE9C392F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -37672,12 +37685,4 @@
     <ds:schemaRef ds:uri="b38e6452-0983-483a-b0d4-324af6d44e4d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A59176D2-D324-41A5-A125-AC358C249804}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
rename 27001 and 27002 tab
</commit_message>
<xml_diff>
--- a/src/assets/database.xlsx
+++ b/src/assets/database.xlsx
@@ -3,15 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E35DF83-8531-4BBD-99D0-42430922D763}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAEDAEB3-D6C6-4DEA-9630-37C389F4CB32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="465" yWindow="480" windowWidth="15165" windowHeight="6795" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ChangeLog" sheetId="11" r:id="rId1"/>
     <sheet name="ISO" sheetId="1" r:id="rId2"/>
     <sheet name="PDPB draft" sheetId="14" r:id="rId3"/>
-    <sheet name="ISO27001+27002" sheetId="15" r:id="rId4"/>
+    <sheet name="27001+27002" sheetId="15" r:id="rId4"/>
     <sheet name="Australia " sheetId="2" r:id="rId5"/>
     <sheet name="Brazil " sheetId="9" r:id="rId6"/>
     <sheet name="California CCPA " sheetId="8" r:id="rId7"/>
@@ -30162,8 +30162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A3C330C-CA93-42D3-B435-3519CA427734}">
   <dimension ref="A1:E199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
-      <selection activeCell="E197" sqref="E197:E199"/>
+    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="C185" sqref="C185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -49925,24 +49925,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_STS_x0020_Hashtags xmlns="b38e6452-0983-483a-b0d4-324af6d44e4d"/>
-    <MediaServiceKeyPoints xmlns="b38e6452-0983-483a-b0d4-324af6d44e4d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010072B72D3E1CFCDD40BC0C6D9CCD45E0BB" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1091b63e79dc81a90741573e3164413c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="759c4387-f01d-437d-8a5d-56d9b05a6914" xmlns:ns4="b38e6452-0983-483a-b0d4-324af6d44e4d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7010e408eae2039b0bc4bac303a742c1" ns3:_="" ns4:_="">
     <xsd:import namespace="759c4387-f01d-437d-8a5d-56d9b05a6914"/>
@@ -50193,25 +50175,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A59176D2-D324-41A5-A125-AC358C249804}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_STS_x0020_Hashtags xmlns="b38e6452-0983-483a-b0d4-324af6d44e4d"/>
+    <MediaServiceKeyPoints xmlns="b38e6452-0983-483a-b0d4-324af6d44e4d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71725466-609F-438E-9D55-68B1CE9C392F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b38e6452-0983-483a-b0d4-324af6d44e4d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC11F96C-E600-42F3-BB18-A579B8C44705}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -50228,4 +50210,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71725466-609F-438E-9D55-68B1CE9C392F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b38e6452-0983-483a-b0d4-324af6d44e4d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A59176D2-D324-41A5-A125-AC358C249804}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fixed reference error from 27002 12.7.1
</commit_message>
<xml_diff>
--- a/src/assets/database.xlsx
+++ b/src/assets/database.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAEDAEB3-D6C6-4DEA-9630-37C389F4CB32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA4F9CA-B277-4221-8781-FA568858F103}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="ChangeLog" sheetId="11" r:id="rId1"/>
     <sheet name="ISO" sheetId="1" r:id="rId2"/>
     <sheet name="PDPB draft" sheetId="14" r:id="rId3"/>
-    <sheet name="27001+27002" sheetId="15" r:id="rId4"/>
+    <sheet name="ISO 27001+27002" sheetId="15" r:id="rId4"/>
     <sheet name="Australia " sheetId="2" r:id="rId5"/>
     <sheet name="Brazil " sheetId="9" r:id="rId6"/>
     <sheet name="California CCPA " sheetId="8" r:id="rId7"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8831" uniqueCount="5184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8831" uniqueCount="5183">
   <si>
     <t>id</t>
   </si>
@@ -17418,9 +17418,6 @@
   </si>
   <si>
     <t>Information systems should be regularly reviewed for compliance with the organization’s information security policies and standards.</t>
-  </si>
-  <si>
-    <t>6.9.7.2</t>
   </si>
 </sst>
 </file>
@@ -30162,8 +30159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A3C330C-CA93-42D3-B435-3519CA427734}">
   <dimension ref="A1:E199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
-      <selection activeCell="C185" sqref="C185"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="E138" sqref="E138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -31973,7 +31970,7 @@
         <v>5012</v>
       </c>
       <c r="E137" t="s">
-        <v>5183</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="138" spans="1:5">
@@ -49925,6 +49922,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_STS_x0020_Hashtags xmlns="b38e6452-0983-483a-b0d4-324af6d44e4d"/>
+    <MediaServiceKeyPoints xmlns="b38e6452-0983-483a-b0d4-324af6d44e4d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010072B72D3E1CFCDD40BC0C6D9CCD45E0BB" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1091b63e79dc81a90741573e3164413c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="759c4387-f01d-437d-8a5d-56d9b05a6914" xmlns:ns4="b38e6452-0983-483a-b0d4-324af6d44e4d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7010e408eae2039b0bc4bac303a742c1" ns3:_="" ns4:_="">
     <xsd:import namespace="759c4387-f01d-437d-8a5d-56d9b05a6914"/>
@@ -50175,25 +50190,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_STS_x0020_Hashtags xmlns="b38e6452-0983-483a-b0d4-324af6d44e4d"/>
-    <MediaServiceKeyPoints xmlns="b38e6452-0983-483a-b0d4-324af6d44e4d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A59176D2-D324-41A5-A125-AC358C249804}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71725466-609F-438E-9D55-68B1CE9C392F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b38e6452-0983-483a-b0d4-324af6d44e4d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC11F96C-E600-42F3-BB18-A579B8C44705}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -50210,22 +50225,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71725466-609F-438E-9D55-68B1CE9C392F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b38e6452-0983-483a-b0d4-324af6d44e4d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A59176D2-D324-41A5-A125-AC358C249804}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>